<commit_message>
Add beginDate as an attribute, as well as actual gals. Added an inter-trip check to see if mpg and price jump excessively between trips.
Fixed typos in data files.
</commit_message>
<xml_diff>
--- a/raw/Red book.xlsx
+++ b/raw/Red book.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="24760" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
-      <selection activeCell="A675" sqref="A675"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="C221" sqref="C221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-12.5</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2989,7 +2989,7 @@
         <v>99570</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3498,7 +3498,7 @@
         <v>15.3</v>
       </c>
       <c r="F61">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G61" t="s">
         <v>16</v>
@@ -11439,7 +11439,7 @@
         <v>52549</v>
       </c>
       <c r="C220">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -13145,10 +13145,10 @@
         <v>1</v>
       </c>
       <c r="E254">
-        <v>1.9</v>
+        <v>19</v>
       </c>
       <c r="F254">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="G254" t="s">
         <v>19</v>
@@ -13695,10 +13695,10 @@
         <v>1</v>
       </c>
       <c r="E265">
-        <v>6.3</v>
+        <v>15.75</v>
       </c>
       <c r="F265">
-        <v>7.25</v>
+        <v>18.13</v>
       </c>
       <c r="G265" t="s">
         <v>19</v>
@@ -15095,10 +15095,12 @@
         <v>1</v>
       </c>
       <c r="E293">
-        <v>4.3</v>
+        <f>15*4.3</f>
+        <v>64.5</v>
       </c>
       <c r="F293">
-        <v>6</v>
+        <f>15*6</f>
+        <v>90</v>
       </c>
       <c r="G293" t="s">
         <v>19</v>
@@ -23947,10 +23949,12 @@
         <v>1</v>
       </c>
       <c r="E470">
-        <v>9.8000000000000007</v>
+        <f>2.5*9.8</f>
+        <v>24.5</v>
       </c>
       <c r="F470">
-        <v>29.38</v>
+        <f>2.5*29.38</f>
+        <v>73.45</v>
       </c>
       <c r="G470" t="s">
         <v>19</v>
@@ -27771,7 +27775,7 @@
         <v>40040</v>
       </c>
       <c r="B549">
-        <v>15755</v>
+        <v>15255</v>
       </c>
       <c r="C549">
         <v>0</v>
@@ -31440,7 +31444,7 @@
         <v>38101</v>
       </c>
       <c r="C627">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D627">
         <v>1</v>
@@ -32762,10 +32766,10 @@
         <v>1</v>
       </c>
       <c r="E655">
-        <v>5.74</v>
+        <v>17.22</v>
       </c>
       <c r="F655">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G655" t="s">
         <v>19</v>
@@ -33705,7 +33709,7 @@
         <v>5.4</v>
       </c>
       <c r="F675">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G675" t="s">
         <v>19</v>
@@ -33978,7 +33982,7 @@
         <v>53303</v>
       </c>
       <c r="C681">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D681">
         <v>1</v>

</xml_diff>

<commit_message>
Fix tire data - required fixing weighted average function (to using floats rather than ints), and fix data file (had ethanol and tire data switched in red book).
</commit_message>
<xml_diff>
--- a/raw/Red book.xlsx
+++ b/raw/Red book.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="24760" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24760" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,10 +100,22 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -124,8 +136,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -135,7 +151,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="C221" sqref="C221"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -18958,10 +18978,10 @@
         <v>19</v>
       </c>
       <c r="H370">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I370">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J370" t="s">
         <v>22</v>
@@ -19008,10 +19028,10 @@
         <v>19</v>
       </c>
       <c r="H371">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I371">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J371" t="s">
         <v>22</v>
@@ -19058,10 +19078,10 @@
         <v>19</v>
       </c>
       <c r="H372">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I372">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J372" t="s">
         <v>22</v>
@@ -19108,10 +19128,10 @@
         <v>19</v>
       </c>
       <c r="H373">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I373">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J373" t="s">
         <v>22</v>
@@ -19158,10 +19178,10 @@
         <v>19</v>
       </c>
       <c r="H374">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I374">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J374" t="s">
         <v>22</v>
@@ -19208,10 +19228,10 @@
         <v>19</v>
       </c>
       <c r="H375">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I375">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J375" t="s">
         <v>22</v>
@@ -19258,10 +19278,10 @@
         <v>19</v>
       </c>
       <c r="H376">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I376">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J376" t="s">
         <v>22</v>
@@ -19308,10 +19328,10 @@
         <v>19</v>
       </c>
       <c r="H377">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I377">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J377" t="s">
         <v>22</v>
@@ -19358,10 +19378,10 @@
         <v>19</v>
       </c>
       <c r="H378">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I378">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J378" t="s">
         <v>22</v>
@@ -19408,10 +19428,10 @@
         <v>19</v>
       </c>
       <c r="H379">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I379">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J379" t="s">
         <v>22</v>
@@ -19458,10 +19478,10 @@
         <v>19</v>
       </c>
       <c r="H380">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I380">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J380" t="s">
         <v>22</v>
@@ -19508,10 +19528,10 @@
         <v>19</v>
       </c>
       <c r="H381">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I381">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J381" t="s">
         <v>22</v>
@@ -19558,10 +19578,10 @@
         <v>19</v>
       </c>
       <c r="H382">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I382">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J382" t="s">
         <v>22</v>
@@ -19608,10 +19628,10 @@
         <v>19</v>
       </c>
       <c r="H383">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I383">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J383" t="s">
         <v>22</v>
@@ -19658,10 +19678,10 @@
         <v>19</v>
       </c>
       <c r="H384">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I384">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J384" t="s">
         <v>22</v>
@@ -19708,10 +19728,10 @@
         <v>19</v>
       </c>
       <c r="H385">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I385">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J385" t="s">
         <v>22</v>
@@ -19758,10 +19778,10 @@
         <v>19</v>
       </c>
       <c r="H386">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I386">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J386" t="s">
         <v>22</v>
@@ -19808,10 +19828,10 @@
         <v>19</v>
       </c>
       <c r="H387">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I387">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J387" t="s">
         <v>22</v>
@@ -19858,10 +19878,10 @@
         <v>19</v>
       </c>
       <c r="H388">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I388">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J388" t="s">
         <v>22</v>
@@ -19908,10 +19928,10 @@
         <v>19</v>
       </c>
       <c r="H389">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I389">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J389" t="s">
         <v>22</v>
@@ -19958,10 +19978,10 @@
         <v>19</v>
       </c>
       <c r="H390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I390">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J390" t="s">
         <v>22</v>
@@ -20008,10 +20028,10 @@
         <v>19</v>
       </c>
       <c r="H391">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I391">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J391" t="s">
         <v>22</v>
@@ -20058,10 +20078,10 @@
         <v>19</v>
       </c>
       <c r="H392">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I392">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J392" t="s">
         <v>22</v>
@@ -20108,10 +20128,10 @@
         <v>19</v>
       </c>
       <c r="H393">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I393">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J393" t="s">
         <v>22</v>
@@ -20158,10 +20178,10 @@
         <v>19</v>
       </c>
       <c r="H394">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J394" t="s">
         <v>22</v>
@@ -20208,10 +20228,10 @@
         <v>19</v>
       </c>
       <c r="H395">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I395">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J395" t="s">
         <v>22</v>
@@ -20258,10 +20278,10 @@
         <v>19</v>
       </c>
       <c r="H396">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I396">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J396" t="s">
         <v>22</v>
@@ -20308,10 +20328,10 @@
         <v>19</v>
       </c>
       <c r="H397">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I397">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J397" t="s">
         <v>22</v>
@@ -20358,10 +20378,10 @@
         <v>19</v>
       </c>
       <c r="H398">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I398">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J398" t="s">
         <v>22</v>
@@ -20408,10 +20428,10 @@
         <v>19</v>
       </c>
       <c r="H399">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I399">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J399" t="s">
         <v>22</v>
@@ -20458,10 +20478,10 @@
         <v>19</v>
       </c>
       <c r="H400">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I400">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J400" t="s">
         <v>22</v>
@@ -20508,10 +20528,10 @@
         <v>19</v>
       </c>
       <c r="H401">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I401">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J401" t="s">
         <v>22</v>
@@ -20558,10 +20578,10 @@
         <v>19</v>
       </c>
       <c r="H402">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I402">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J402" t="s">
         <v>22</v>
@@ -20608,10 +20628,10 @@
         <v>19</v>
       </c>
       <c r="H403">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I403">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J403" t="s">
         <v>22</v>
@@ -20658,10 +20678,10 @@
         <v>19</v>
       </c>
       <c r="H404">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I404">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J404" t="s">
         <v>22</v>
@@ -20708,10 +20728,10 @@
         <v>19</v>
       </c>
       <c r="H405">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I405">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J405" t="s">
         <v>22</v>
@@ -20758,10 +20778,10 @@
         <v>19</v>
       </c>
       <c r="H406">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I406">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J406" t="s">
         <v>22</v>
@@ -20808,10 +20828,10 @@
         <v>19</v>
       </c>
       <c r="H407">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I407">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J407" t="s">
         <v>22</v>
@@ -20858,10 +20878,10 @@
         <v>19</v>
       </c>
       <c r="H408">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I408">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J408" t="s">
         <v>22</v>
@@ -20908,10 +20928,10 @@
         <v>19</v>
       </c>
       <c r="H409">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I409">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J409" t="s">
         <v>22</v>
@@ -20958,10 +20978,10 @@
         <v>19</v>
       </c>
       <c r="H410">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I410">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J410" t="s">
         <v>22</v>
@@ -21008,10 +21028,10 @@
         <v>19</v>
       </c>
       <c r="H411">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I411">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J411" t="s">
         <v>22</v>
@@ -21058,10 +21078,10 @@
         <v>19</v>
       </c>
       <c r="H412">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I412">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J412" t="s">
         <v>22</v>
@@ -21108,10 +21128,10 @@
         <v>19</v>
       </c>
       <c r="H413">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I413">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J413" t="s">
         <v>22</v>
@@ -21158,10 +21178,10 @@
         <v>19</v>
       </c>
       <c r="H414">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I414">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J414" t="s">
         <v>22</v>
@@ -21208,10 +21228,10 @@
         <v>19</v>
       </c>
       <c r="H415">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I415">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J415" t="s">
         <v>22</v>
@@ -21258,10 +21278,10 @@
         <v>19</v>
       </c>
       <c r="H416">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I416">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J416" t="s">
         <v>22</v>
@@ -21308,10 +21328,10 @@
         <v>19</v>
       </c>
       <c r="H417">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I417">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J417" t="s">
         <v>22</v>
@@ -21358,10 +21378,10 @@
         <v>19</v>
       </c>
       <c r="H418">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I418">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J418" t="s">
         <v>22</v>
@@ -21408,10 +21428,10 @@
         <v>19</v>
       </c>
       <c r="H419">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I419">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J419" t="s">
         <v>22</v>
@@ -21458,10 +21478,10 @@
         <v>19</v>
       </c>
       <c r="H420">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I420">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J420" t="s">
         <v>22</v>
@@ -21508,10 +21528,10 @@
         <v>19</v>
       </c>
       <c r="H421">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I421">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J421" t="s">
         <v>22</v>
@@ -21558,10 +21578,10 @@
         <v>19</v>
       </c>
       <c r="H422">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I422">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J422" t="s">
         <v>22</v>
@@ -21608,10 +21628,10 @@
         <v>19</v>
       </c>
       <c r="H423">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I423">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J423" t="s">
         <v>22</v>
@@ -21658,10 +21678,10 @@
         <v>19</v>
       </c>
       <c r="H424">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I424">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J424" t="s">
         <v>22</v>
@@ -21708,10 +21728,10 @@
         <v>19</v>
       </c>
       <c r="H425">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I425">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J425" t="s">
         <v>22</v>
@@ -21758,10 +21778,10 @@
         <v>19</v>
       </c>
       <c r="H426">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I426">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J426" t="s">
         <v>22</v>
@@ -21808,10 +21828,10 @@
         <v>19</v>
       </c>
       <c r="H427">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I427">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J427" t="s">
         <v>22</v>
@@ -21858,10 +21878,10 @@
         <v>19</v>
       </c>
       <c r="H428">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I428">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J428" t="s">
         <v>22</v>
@@ -21908,10 +21928,10 @@
         <v>19</v>
       </c>
       <c r="H429">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I429">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J429" t="s">
         <v>22</v>
@@ -21958,10 +21978,10 @@
         <v>19</v>
       </c>
       <c r="H430">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I430">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J430" t="s">
         <v>22</v>
@@ -22008,10 +22028,10 @@
         <v>19</v>
       </c>
       <c r="H431">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I431">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J431" t="s">
         <v>22</v>
@@ -22058,10 +22078,10 @@
         <v>19</v>
       </c>
       <c r="H432">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I432">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J432" t="s">
         <v>22</v>
@@ -22108,10 +22128,10 @@
         <v>19</v>
       </c>
       <c r="H433">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I433">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J433" t="s">
         <v>22</v>
@@ -22158,10 +22178,10 @@
         <v>19</v>
       </c>
       <c r="H434">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I434">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J434" t="s">
         <v>22</v>
@@ -22208,10 +22228,10 @@
         <v>19</v>
       </c>
       <c r="H435">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I435">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J435" t="s">
         <v>22</v>
@@ -22258,10 +22278,10 @@
         <v>19</v>
       </c>
       <c r="H436">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I436">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J436" t="s">
         <v>22</v>
@@ -22308,10 +22328,10 @@
         <v>19</v>
       </c>
       <c r="H437">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I437">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J437" t="s">
         <v>22</v>
@@ -22358,10 +22378,10 @@
         <v>19</v>
       </c>
       <c r="H438">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I438">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J438" t="s">
         <v>22</v>
@@ -22408,10 +22428,10 @@
         <v>19</v>
       </c>
       <c r="H439">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I439">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J439" t="s">
         <v>22</v>
@@ -22458,10 +22478,10 @@
         <v>19</v>
       </c>
       <c r="H440">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I440">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J440" t="s">
         <v>22</v>
@@ -22508,10 +22528,10 @@
         <v>19</v>
       </c>
       <c r="H441">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I441">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J441" t="s">
         <v>22</v>
@@ -22558,10 +22578,10 @@
         <v>19</v>
       </c>
       <c r="H442">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I442">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J442" t="s">
         <v>22</v>
@@ -22608,10 +22628,10 @@
         <v>19</v>
       </c>
       <c r="H443">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I443">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J443" t="s">
         <v>22</v>
@@ -22658,10 +22678,10 @@
         <v>19</v>
       </c>
       <c r="H444">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I444">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J444" t="s">
         <v>22</v>
@@ -22708,10 +22728,10 @@
         <v>19</v>
       </c>
       <c r="H445">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I445">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J445" t="s">
         <v>22</v>
@@ -22758,10 +22778,10 @@
         <v>19</v>
       </c>
       <c r="H446">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I446">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J446" t="s">
         <v>22</v>
@@ -22808,10 +22828,10 @@
         <v>19</v>
       </c>
       <c r="H447">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I447">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J447" t="s">
         <v>22</v>
@@ -22858,10 +22878,10 @@
         <v>19</v>
       </c>
       <c r="H448">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I448">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J448" t="s">
         <v>22</v>
@@ -22908,10 +22928,10 @@
         <v>19</v>
       </c>
       <c r="H449">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I449">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J449" t="s">
         <v>22</v>
@@ -22958,10 +22978,10 @@
         <v>19</v>
       </c>
       <c r="H450">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I450">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J450" t="s">
         <v>22</v>
@@ -23008,10 +23028,10 @@
         <v>19</v>
       </c>
       <c r="H451">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I451">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J451" t="s">
         <v>22</v>
@@ -23058,10 +23078,10 @@
         <v>19</v>
       </c>
       <c r="H452">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I452">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J452" t="s">
         <v>22</v>
@@ -23108,10 +23128,10 @@
         <v>19</v>
       </c>
       <c r="H453">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I453">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J453" t="s">
         <v>22</v>
@@ -23158,10 +23178,10 @@
         <v>19</v>
       </c>
       <c r="H454">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I454">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J454" t="s">
         <v>22</v>
@@ -23208,10 +23228,10 @@
         <v>19</v>
       </c>
       <c r="H455">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I455">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J455" t="s">
         <v>22</v>
@@ -23258,10 +23278,10 @@
         <v>19</v>
       </c>
       <c r="H456">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I456">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J456" t="s">
         <v>22</v>
@@ -23308,10 +23328,10 @@
         <v>19</v>
       </c>
       <c r="H457">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I457">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J457" t="s">
         <v>22</v>
@@ -23358,10 +23378,10 @@
         <v>19</v>
       </c>
       <c r="H458">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I458">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J458" t="s">
         <v>22</v>
@@ -23408,10 +23428,10 @@
         <v>19</v>
       </c>
       <c r="H459">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I459">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J459" t="s">
         <v>22</v>
@@ -23458,10 +23478,10 @@
         <v>19</v>
       </c>
       <c r="H460">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I460">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J460" t="s">
         <v>22</v>
@@ -23508,10 +23528,10 @@
         <v>19</v>
       </c>
       <c r="H461">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I461">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J461" t="s">
         <v>22</v>
@@ -23558,10 +23578,10 @@
         <v>19</v>
       </c>
       <c r="H462">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I462">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J462" t="s">
         <v>22</v>
@@ -23608,10 +23628,10 @@
         <v>19</v>
       </c>
       <c r="H463">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I463">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J463" t="s">
         <v>22</v>
@@ -23658,10 +23678,10 @@
         <v>19</v>
       </c>
       <c r="H464">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I464">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J464" t="s">
         <v>22</v>
@@ -23708,10 +23728,10 @@
         <v>19</v>
       </c>
       <c r="H465">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I465">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J465" t="s">
         <v>22</v>
@@ -23758,10 +23778,10 @@
         <v>19</v>
       </c>
       <c r="H466">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I466">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J466" t="s">
         <v>22</v>
@@ -23808,10 +23828,10 @@
         <v>19</v>
       </c>
       <c r="H467">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I467">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J467" t="s">
         <v>22</v>
@@ -23858,10 +23878,10 @@
         <v>19</v>
       </c>
       <c r="H468">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I468">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J468" t="s">
         <v>22</v>
@@ -23908,10 +23928,10 @@
         <v>19</v>
       </c>
       <c r="H469">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I469">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J469" t="s">
         <v>22</v>
@@ -23960,10 +23980,10 @@
         <v>19</v>
       </c>
       <c r="H470">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I470">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J470" t="s">
         <v>22</v>
@@ -24010,10 +24030,10 @@
         <v>19</v>
       </c>
       <c r="H471">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I471">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J471" t="s">
         <v>22</v>
@@ -24060,10 +24080,10 @@
         <v>19</v>
       </c>
       <c r="H472">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I472">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J472" t="s">
         <v>22</v>
@@ -24110,10 +24130,10 @@
         <v>19</v>
       </c>
       <c r="H473">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I473">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J473" t="s">
         <v>22</v>
@@ -24160,10 +24180,10 @@
         <v>19</v>
       </c>
       <c r="H474">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I474">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J474" t="s">
         <v>22</v>
@@ -24210,10 +24230,10 @@
         <v>19</v>
       </c>
       <c r="H475">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I475">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J475" t="s">
         <v>22</v>
@@ -24260,10 +24280,10 @@
         <v>19</v>
       </c>
       <c r="H476">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I476">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J476" t="s">
         <v>22</v>
@@ -24310,10 +24330,10 @@
         <v>19</v>
       </c>
       <c r="H477">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I477">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J477" t="s">
         <v>22</v>
@@ -24360,10 +24380,10 @@
         <v>19</v>
       </c>
       <c r="H478">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I478">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J478" t="s">
         <v>22</v>
@@ -24410,10 +24430,10 @@
         <v>19</v>
       </c>
       <c r="H479">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I479">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J479" t="s">
         <v>22</v>
@@ -24460,10 +24480,10 @@
         <v>19</v>
       </c>
       <c r="H480">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I480">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J480" t="s">
         <v>22</v>
@@ -24510,10 +24530,10 @@
         <v>19</v>
       </c>
       <c r="H481">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I481">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J481" t="s">
         <v>22</v>
@@ -24560,10 +24580,10 @@
         <v>19</v>
       </c>
       <c r="H482">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I482">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J482" t="s">
         <v>22</v>
@@ -24610,10 +24630,10 @@
         <v>19</v>
       </c>
       <c r="H483">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I483">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J483" t="s">
         <v>22</v>
@@ -24660,10 +24680,10 @@
         <v>19</v>
       </c>
       <c r="H484">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I484">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J484" t="s">
         <v>22</v>
@@ -24710,10 +24730,10 @@
         <v>19</v>
       </c>
       <c r="H485">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I485">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J485" t="s">
         <v>22</v>
@@ -24760,10 +24780,10 @@
         <v>19</v>
       </c>
       <c r="H486">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I486">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J486" t="s">
         <v>22</v>
@@ -24810,10 +24830,10 @@
         <v>19</v>
       </c>
       <c r="H487">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I487">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J487" t="s">
         <v>22</v>
@@ -24860,10 +24880,10 @@
         <v>19</v>
       </c>
       <c r="H488">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I488">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J488" t="s">
         <v>22</v>
@@ -24910,10 +24930,10 @@
         <v>19</v>
       </c>
       <c r="H489">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I489">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J489" t="s">
         <v>22</v>
@@ -24960,10 +24980,10 @@
         <v>19</v>
       </c>
       <c r="H490">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I490">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J490" t="s">
         <v>22</v>
@@ -25010,10 +25030,10 @@
         <v>19</v>
       </c>
       <c r="H491">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I491">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J491" t="s">
         <v>22</v>
@@ -25060,10 +25080,10 @@
         <v>19</v>
       </c>
       <c r="H492">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I492">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J492" t="s">
         <v>22</v>
@@ -25110,10 +25130,10 @@
         <v>19</v>
       </c>
       <c r="H493">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I493">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J493" t="s">
         <v>22</v>
@@ -25160,10 +25180,10 @@
         <v>19</v>
       </c>
       <c r="H494">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I494">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J494" t="s">
         <v>22</v>
@@ -25210,10 +25230,10 @@
         <v>19</v>
       </c>
       <c r="H495">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I495">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J495" t="s">
         <v>22</v>
@@ -25260,10 +25280,10 @@
         <v>19</v>
       </c>
       <c r="H496">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I496">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J496" t="s">
         <v>22</v>
@@ -25310,10 +25330,10 @@
         <v>19</v>
       </c>
       <c r="H497">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I497">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J497" t="s">
         <v>22</v>
@@ -25360,10 +25380,10 @@
         <v>19</v>
       </c>
       <c r="H498">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I498">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J498" t="s">
         <v>22</v>
@@ -25410,10 +25430,10 @@
         <v>19</v>
       </c>
       <c r="H499">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I499">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J499" t="s">
         <v>22</v>
@@ -25460,10 +25480,10 @@
         <v>19</v>
       </c>
       <c r="H500">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I500">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J500" t="s">
         <v>22</v>
@@ -25510,10 +25530,10 @@
         <v>19</v>
       </c>
       <c r="H501">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I501">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J501" t="s">
         <v>22</v>
@@ -25560,10 +25580,10 @@
         <v>19</v>
       </c>
       <c r="H502">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I502">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J502" t="s">
         <v>22</v>
@@ -25610,10 +25630,10 @@
         <v>19</v>
       </c>
       <c r="H503">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I503">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J503" t="s">
         <v>22</v>
@@ -25660,10 +25680,10 @@
         <v>19</v>
       </c>
       <c r="H504">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I504">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J504" t="s">
         <v>22</v>
@@ -25710,10 +25730,10 @@
         <v>19</v>
       </c>
       <c r="H505">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I505">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J505" t="s">
         <v>22</v>
@@ -25760,10 +25780,10 @@
         <v>19</v>
       </c>
       <c r="H506">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I506">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J506" t="s">
         <v>22</v>
@@ -25810,10 +25830,10 @@
         <v>19</v>
       </c>
       <c r="H507">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I507">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J507" t="s">
         <v>22</v>
@@ -25860,10 +25880,10 @@
         <v>19</v>
       </c>
       <c r="H508">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I508">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J508" t="s">
         <v>22</v>
@@ -25910,10 +25930,10 @@
         <v>19</v>
       </c>
       <c r="H509">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I509">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J509" t="s">
         <v>22</v>
@@ -25960,10 +25980,10 @@
         <v>19</v>
       </c>
       <c r="H510">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I510">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J510" t="s">
         <v>22</v>
@@ -26007,10 +26027,10 @@
         <v>19</v>
       </c>
       <c r="H511">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I511">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J511" t="s">
         <v>22</v>
@@ -26054,10 +26074,10 @@
         <v>19</v>
       </c>
       <c r="H512">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I512">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J512" t="s">
         <v>22</v>
@@ -26101,10 +26121,10 @@
         <v>19</v>
       </c>
       <c r="H513">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I513">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J513" t="s">
         <v>22</v>
@@ -26148,10 +26168,10 @@
         <v>19</v>
       </c>
       <c r="H514">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I514">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J514" t="s">
         <v>22</v>
@@ -26195,10 +26215,10 @@
         <v>19</v>
       </c>
       <c r="H515">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I515">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J515" t="s">
         <v>22</v>
@@ -26242,10 +26262,10 @@
         <v>19</v>
       </c>
       <c r="H516">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I516">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J516" t="s">
         <v>22</v>
@@ -26289,10 +26309,10 @@
         <v>19</v>
       </c>
       <c r="H517">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I517">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J517" t="s">
         <v>22</v>
@@ -26336,10 +26356,10 @@
         <v>19</v>
       </c>
       <c r="H518">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I518">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J518" t="s">
         <v>22</v>
@@ -26383,10 +26403,10 @@
         <v>19</v>
       </c>
       <c r="H519">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I519">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J519" t="s">
         <v>22</v>
@@ -26430,10 +26450,10 @@
         <v>19</v>
       </c>
       <c r="H520">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I520">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J520" t="s">
         <v>22</v>
@@ -26477,10 +26497,10 @@
         <v>19</v>
       </c>
       <c r="H521">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I521">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J521" t="s">
         <v>22</v>
@@ -26524,10 +26544,10 @@
         <v>19</v>
       </c>
       <c r="H522">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I522">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J522" t="s">
         <v>22</v>
@@ -26571,10 +26591,10 @@
         <v>19</v>
       </c>
       <c r="H523">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I523">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J523" t="s">
         <v>22</v>
@@ -26618,10 +26638,10 @@
         <v>19</v>
       </c>
       <c r="H524">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I524">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J524" t="s">
         <v>22</v>
@@ -26665,10 +26685,10 @@
         <v>19</v>
       </c>
       <c r="H525">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I525">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J525" t="s">
         <v>22</v>
@@ -26712,10 +26732,10 @@
         <v>19</v>
       </c>
       <c r="H526">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I526">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J526" t="s">
         <v>22</v>
@@ -26759,10 +26779,10 @@
         <v>19</v>
       </c>
       <c r="H527">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I527">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J527" t="s">
         <v>22</v>
@@ -26806,10 +26826,10 @@
         <v>19</v>
       </c>
       <c r="H528">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I528">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J528" t="s">
         <v>22</v>
@@ -26853,10 +26873,10 @@
         <v>19</v>
       </c>
       <c r="H529">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I529">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J529" t="s">
         <v>22</v>
@@ -26900,10 +26920,10 @@
         <v>19</v>
       </c>
       <c r="H530">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I530">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J530" t="s">
         <v>22</v>
@@ -26947,10 +26967,10 @@
         <v>19</v>
       </c>
       <c r="H531">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I531">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J531" t="s">
         <v>22</v>
@@ -26994,10 +27014,10 @@
         <v>19</v>
       </c>
       <c r="H532">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I532">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J532" t="s">
         <v>22</v>
@@ -27041,10 +27061,10 @@
         <v>19</v>
       </c>
       <c r="H533">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I533">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J533" t="s">
         <v>22</v>
@@ -27088,10 +27108,10 @@
         <v>19</v>
       </c>
       <c r="H534">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I534">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J534" t="s">
         <v>22</v>
@@ -27135,10 +27155,10 @@
         <v>19</v>
       </c>
       <c r="H535">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I535">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J535" t="s">
         <v>22</v>
@@ -27182,10 +27202,10 @@
         <v>19</v>
       </c>
       <c r="H536">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I536">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J536" t="s">
         <v>22</v>
@@ -27229,10 +27249,10 @@
         <v>19</v>
       </c>
       <c r="H537">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I537">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J537" t="s">
         <v>22</v>
@@ -27276,10 +27296,10 @@
         <v>19</v>
       </c>
       <c r="H538">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I538">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J538" t="s">
         <v>22</v>
@@ -27323,10 +27343,10 @@
         <v>19</v>
       </c>
       <c r="H539">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I539">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J539" t="s">
         <v>22</v>
@@ -27370,10 +27390,10 @@
         <v>19</v>
       </c>
       <c r="H540">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I540">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J540" t="s">
         <v>22</v>
@@ -27417,10 +27437,10 @@
         <v>19</v>
       </c>
       <c r="H541">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I541">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J541" t="s">
         <v>22</v>
@@ -27464,10 +27484,10 @@
         <v>19</v>
       </c>
       <c r="H542">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I542">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J542" t="s">
         <v>22</v>
@@ -27511,10 +27531,10 @@
         <v>19</v>
       </c>
       <c r="H543">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I543">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J543" t="s">
         <v>22</v>
@@ -27558,10 +27578,10 @@
         <v>19</v>
       </c>
       <c r="H544">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I544">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J544" t="s">
         <v>22</v>
@@ -27605,10 +27625,10 @@
         <v>19</v>
       </c>
       <c r="H545">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I545">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J545" t="s">
         <v>22</v>
@@ -27652,10 +27672,10 @@
         <v>19</v>
       </c>
       <c r="H546">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I546">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J546" t="s">
         <v>22</v>
@@ -27699,10 +27719,10 @@
         <v>19</v>
       </c>
       <c r="H547">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I547">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J547" t="s">
         <v>22</v>
@@ -27746,10 +27766,10 @@
         <v>19</v>
       </c>
       <c r="H548">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I548">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J548" t="s">
         <v>22</v>
@@ -27793,10 +27813,10 @@
         <v>19</v>
       </c>
       <c r="H549">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I549">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J549" t="s">
         <v>22</v>
@@ -27840,10 +27860,10 @@
         <v>19</v>
       </c>
       <c r="H550">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I550">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J550" t="s">
         <v>22</v>
@@ -27887,10 +27907,10 @@
         <v>19</v>
       </c>
       <c r="H551">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I551">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J551" t="s">
         <v>22</v>
@@ -27934,10 +27954,10 @@
         <v>19</v>
       </c>
       <c r="H552">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I552">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J552" t="s">
         <v>22</v>
@@ -27981,10 +28001,10 @@
         <v>19</v>
       </c>
       <c r="H553">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I553">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J553" t="s">
         <v>22</v>
@@ -28028,10 +28048,10 @@
         <v>19</v>
       </c>
       <c r="H554">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I554">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J554" t="s">
         <v>22</v>
@@ -28075,10 +28095,10 @@
         <v>19</v>
       </c>
       <c r="H555">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I555">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J555" t="s">
         <v>22</v>
@@ -28122,10 +28142,10 @@
         <v>19</v>
       </c>
       <c r="H556">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I556">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J556" t="s">
         <v>22</v>
@@ -28169,10 +28189,10 @@
         <v>19</v>
       </c>
       <c r="H557">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I557">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J557" t="s">
         <v>22</v>
@@ -28216,10 +28236,10 @@
         <v>19</v>
       </c>
       <c r="H558">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I558">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J558" t="s">
         <v>22</v>
@@ -28263,10 +28283,10 @@
         <v>19</v>
       </c>
       <c r="H559">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I559">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J559" t="s">
         <v>22</v>
@@ -28310,10 +28330,10 @@
         <v>19</v>
       </c>
       <c r="H560">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I560">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J560" t="s">
         <v>22</v>
@@ -28357,10 +28377,10 @@
         <v>19</v>
       </c>
       <c r="H561">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I561">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J561" t="s">
         <v>22</v>
@@ -28404,10 +28424,10 @@
         <v>19</v>
       </c>
       <c r="H562">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I562">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J562" t="s">
         <v>22</v>
@@ -28451,10 +28471,10 @@
         <v>19</v>
       </c>
       <c r="H563">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I563">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J563" t="s">
         <v>22</v>
@@ -28498,10 +28518,10 @@
         <v>19</v>
       </c>
       <c r="H564">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I564">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J564" t="s">
         <v>22</v>
@@ -28545,10 +28565,10 @@
         <v>19</v>
       </c>
       <c r="H565">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I565">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J565" t="s">
         <v>22</v>
@@ -28592,10 +28612,10 @@
         <v>19</v>
       </c>
       <c r="H566">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I566">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J566" t="s">
         <v>22</v>
@@ -28639,10 +28659,10 @@
         <v>19</v>
       </c>
       <c r="H567">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I567">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J567" t="s">
         <v>22</v>
@@ -28686,10 +28706,10 @@
         <v>19</v>
       </c>
       <c r="H568">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I568">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J568" t="s">
         <v>22</v>
@@ -28733,10 +28753,10 @@
         <v>19</v>
       </c>
       <c r="H569">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I569">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J569" t="s">
         <v>22</v>
@@ -28780,10 +28800,10 @@
         <v>19</v>
       </c>
       <c r="H570">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I570">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J570" t="s">
         <v>22</v>
@@ -28827,10 +28847,10 @@
         <v>19</v>
       </c>
       <c r="H571">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I571">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J571" t="s">
         <v>22</v>
@@ -28874,10 +28894,10 @@
         <v>19</v>
       </c>
       <c r="H572">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I572">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J572" t="s">
         <v>22</v>
@@ -28921,10 +28941,10 @@
         <v>19</v>
       </c>
       <c r="H573">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I573">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J573" t="s">
         <v>22</v>
@@ -28968,10 +28988,10 @@
         <v>19</v>
       </c>
       <c r="H574">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I574">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J574" t="s">
         <v>22</v>
@@ -29015,10 +29035,10 @@
         <v>19</v>
       </c>
       <c r="H575">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I575">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J575" t="s">
         <v>22</v>
@@ -29062,10 +29082,10 @@
         <v>19</v>
       </c>
       <c r="H576">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I576">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J576" t="s">
         <v>22</v>
@@ -29109,10 +29129,10 @@
         <v>19</v>
       </c>
       <c r="H577">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I577">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J577" t="s">
         <v>22</v>
@@ -29156,10 +29176,10 @@
         <v>19</v>
       </c>
       <c r="H578">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I578">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J578" t="s">
         <v>22</v>
@@ -29203,10 +29223,10 @@
         <v>19</v>
       </c>
       <c r="H579">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I579">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J579" t="s">
         <v>22</v>
@@ -29250,10 +29270,10 @@
         <v>19</v>
       </c>
       <c r="H580">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I580">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J580" t="s">
         <v>22</v>
@@ -29297,10 +29317,10 @@
         <v>19</v>
       </c>
       <c r="H581">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I581">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J581" t="s">
         <v>22</v>
@@ -29344,10 +29364,10 @@
         <v>19</v>
       </c>
       <c r="H582">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I582">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J582" t="s">
         <v>22</v>
@@ -29391,10 +29411,10 @@
         <v>19</v>
       </c>
       <c r="H583">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I583">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J583" t="s">
         <v>22</v>
@@ -29438,10 +29458,10 @@
         <v>19</v>
       </c>
       <c r="H584">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I584">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J584" t="s">
         <v>22</v>
@@ -29485,10 +29505,10 @@
         <v>19</v>
       </c>
       <c r="H585">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I585">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J585" t="s">
         <v>22</v>
@@ -29532,10 +29552,10 @@
         <v>19</v>
       </c>
       <c r="H586">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I586">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J586" t="s">
         <v>22</v>
@@ -29579,10 +29599,10 @@
         <v>19</v>
       </c>
       <c r="H587">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I587">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J587" t="s">
         <v>22</v>
@@ -29626,10 +29646,10 @@
         <v>19</v>
       </c>
       <c r="H588">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I588">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J588" t="s">
         <v>22</v>
@@ -29673,10 +29693,10 @@
         <v>19</v>
       </c>
       <c r="H589">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I589">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J589" t="s">
         <v>22</v>
@@ -29720,10 +29740,10 @@
         <v>19</v>
       </c>
       <c r="H590">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I590">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J590" t="s">
         <v>22</v>
@@ -29767,10 +29787,10 @@
         <v>19</v>
       </c>
       <c r="H591">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I591">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J591" t="s">
         <v>22</v>
@@ -29814,10 +29834,10 @@
         <v>19</v>
       </c>
       <c r="H592">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I592">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J592" t="s">
         <v>22</v>
@@ -29861,10 +29881,10 @@
         <v>19</v>
       </c>
       <c r="H593">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I593">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J593" t="s">
         <v>22</v>
@@ -29908,10 +29928,10 @@
         <v>19</v>
       </c>
       <c r="H594">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I594">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J594" t="s">
         <v>22</v>
@@ -29955,10 +29975,10 @@
         <v>19</v>
       </c>
       <c r="H595">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I595">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J595" t="s">
         <v>22</v>
@@ -30002,10 +30022,10 @@
         <v>19</v>
       </c>
       <c r="H596">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I596">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J596" t="s">
         <v>22</v>
@@ -30049,10 +30069,10 @@
         <v>19</v>
       </c>
       <c r="H597">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I597">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J597" t="s">
         <v>22</v>
@@ -30096,10 +30116,10 @@
         <v>19</v>
       </c>
       <c r="H598">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I598">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J598" t="s">
         <v>22</v>
@@ -30143,10 +30163,10 @@
         <v>19</v>
       </c>
       <c r="H599">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I599">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J599" t="s">
         <v>22</v>
@@ -30190,10 +30210,10 @@
         <v>19</v>
       </c>
       <c r="H600">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I600">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J600" t="s">
         <v>22</v>
@@ -30237,10 +30257,10 @@
         <v>19</v>
       </c>
       <c r="H601">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I601">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J601" t="s">
         <v>22</v>
@@ -30284,10 +30304,10 @@
         <v>19</v>
       </c>
       <c r="H602">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I602">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J602" t="s">
         <v>22</v>
@@ -30331,10 +30351,10 @@
         <v>19</v>
       </c>
       <c r="H603">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I603">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J603" t="s">
         <v>22</v>
@@ -30378,10 +30398,10 @@
         <v>19</v>
       </c>
       <c r="H604">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I604">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J604" t="s">
         <v>22</v>
@@ -30425,10 +30445,10 @@
         <v>19</v>
       </c>
       <c r="H605">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I605">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J605" t="s">
         <v>22</v>
@@ -30472,10 +30492,10 @@
         <v>19</v>
       </c>
       <c r="H606">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I606">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J606" t="s">
         <v>22</v>
@@ -30519,10 +30539,10 @@
         <v>19</v>
       </c>
       <c r="H607">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I607">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J607" t="s">
         <v>22</v>
@@ -30566,10 +30586,10 @@
         <v>19</v>
       </c>
       <c r="H608">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I608">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J608" t="s">
         <v>22</v>
@@ -30613,10 +30633,10 @@
         <v>19</v>
       </c>
       <c r="H609">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I609">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J609" t="s">
         <v>22</v>
@@ -30660,10 +30680,10 @@
         <v>19</v>
       </c>
       <c r="H610">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I610">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J610" t="s">
         <v>22</v>
@@ -30707,10 +30727,10 @@
         <v>19</v>
       </c>
       <c r="H611">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I611">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J611" t="s">
         <v>22</v>
@@ -30754,10 +30774,10 @@
         <v>19</v>
       </c>
       <c r="H612">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I612">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J612" t="s">
         <v>22</v>
@@ -30801,10 +30821,10 @@
         <v>19</v>
       </c>
       <c r="H613">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I613">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J613" t="s">
         <v>22</v>
@@ -30848,10 +30868,10 @@
         <v>19</v>
       </c>
       <c r="H614">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I614">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J614" t="s">
         <v>22</v>
@@ -30895,10 +30915,10 @@
         <v>19</v>
       </c>
       <c r="H615">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I615">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J615" t="s">
         <v>22</v>
@@ -30942,10 +30962,10 @@
         <v>19</v>
       </c>
       <c r="H616">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I616">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J616" t="s">
         <v>22</v>
@@ -30989,10 +31009,10 @@
         <v>19</v>
       </c>
       <c r="H617">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I617">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J617" t="s">
         <v>22</v>
@@ -31036,10 +31056,10 @@
         <v>19</v>
       </c>
       <c r="H618">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I618">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J618" t="s">
         <v>22</v>
@@ -31083,10 +31103,10 @@
         <v>19</v>
       </c>
       <c r="H619">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I619">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J619" t="s">
         <v>22</v>
@@ -31130,10 +31150,10 @@
         <v>19</v>
       </c>
       <c r="H620">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I620">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J620" t="s">
         <v>22</v>
@@ -31177,10 +31197,10 @@
         <v>19</v>
       </c>
       <c r="H621">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I621">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J621" t="s">
         <v>22</v>
@@ -31224,10 +31244,10 @@
         <v>19</v>
       </c>
       <c r="H622">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I622">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J622" t="s">
         <v>22</v>
@@ -31271,10 +31291,10 @@
         <v>19</v>
       </c>
       <c r="H623">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I623">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J623" t="s">
         <v>22</v>
@@ -31318,10 +31338,10 @@
         <v>19</v>
       </c>
       <c r="H624">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I624">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J624" t="s">
         <v>22</v>
@@ -31365,10 +31385,10 @@
         <v>19</v>
       </c>
       <c r="H625">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I625">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J625" t="s">
         <v>22</v>
@@ -31412,10 +31432,10 @@
         <v>19</v>
       </c>
       <c r="H626">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I626">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J626" t="s">
         <v>22</v>
@@ -31459,10 +31479,10 @@
         <v>19</v>
       </c>
       <c r="H627">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I627">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J627" t="s">
         <v>22</v>
@@ -31506,10 +31526,10 @@
         <v>19</v>
       </c>
       <c r="H628">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I628">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J628" t="s">
         <v>22</v>
@@ -31553,10 +31573,10 @@
         <v>19</v>
       </c>
       <c r="H629">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I629">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J629" t="s">
         <v>22</v>
@@ -31600,10 +31620,10 @@
         <v>19</v>
       </c>
       <c r="H630">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I630">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J630" t="s">
         <v>22</v>
@@ -31647,10 +31667,10 @@
         <v>19</v>
       </c>
       <c r="H631">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I631">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J631" t="s">
         <v>22</v>
@@ -31694,10 +31714,10 @@
         <v>19</v>
       </c>
       <c r="H632">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I632">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J632" t="s">
         <v>22</v>
@@ -31741,10 +31761,10 @@
         <v>19</v>
       </c>
       <c r="H633">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I633">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J633" t="s">
         <v>22</v>
@@ -31788,10 +31808,10 @@
         <v>19</v>
       </c>
       <c r="H634">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I634">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J634" t="s">
         <v>22</v>
@@ -31835,10 +31855,10 @@
         <v>19</v>
       </c>
       <c r="H635">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I635">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J635" t="s">
         <v>22</v>
@@ -31882,10 +31902,10 @@
         <v>19</v>
       </c>
       <c r="H636">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I636">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J636" t="s">
         <v>22</v>
@@ -31929,10 +31949,10 @@
         <v>19</v>
       </c>
       <c r="H637">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I637">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J637" t="s">
         <v>22</v>
@@ -31976,10 +31996,10 @@
         <v>19</v>
       </c>
       <c r="H638">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I638">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J638" t="s">
         <v>22</v>
@@ -32023,10 +32043,10 @@
         <v>19</v>
       </c>
       <c r="H639">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I639">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J639" t="s">
         <v>22</v>
@@ -32070,10 +32090,10 @@
         <v>19</v>
       </c>
       <c r="H640">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I640">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J640" t="s">
         <v>22</v>
@@ -32117,10 +32137,10 @@
         <v>19</v>
       </c>
       <c r="H641">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I641">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J641" t="s">
         <v>22</v>
@@ -32164,10 +32184,10 @@
         <v>19</v>
       </c>
       <c r="H642">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I642">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J642" t="s">
         <v>22</v>
@@ -32211,10 +32231,10 @@
         <v>19</v>
       </c>
       <c r="H643">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I643">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J643" t="s">
         <v>22</v>
@@ -32258,10 +32278,10 @@
         <v>19</v>
       </c>
       <c r="H644">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I644">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J644" t="s">
         <v>22</v>
@@ -32305,10 +32325,10 @@
         <v>19</v>
       </c>
       <c r="H645">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I645">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J645" t="s">
         <v>22</v>
@@ -32352,10 +32372,10 @@
         <v>19</v>
       </c>
       <c r="H646">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I646">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J646" t="s">
         <v>22</v>
@@ -32399,10 +32419,10 @@
         <v>19</v>
       </c>
       <c r="H647">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I647">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J647" t="s">
         <v>22</v>
@@ -32446,10 +32466,10 @@
         <v>19</v>
       </c>
       <c r="H648">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I648">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J648" t="s">
         <v>22</v>
@@ -32493,10 +32513,10 @@
         <v>19</v>
       </c>
       <c r="H649">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I649">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J649" t="s">
         <v>22</v>
@@ -32540,10 +32560,10 @@
         <v>19</v>
       </c>
       <c r="H650">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I650">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J650" t="s">
         <v>22</v>
@@ -32587,10 +32607,10 @@
         <v>19</v>
       </c>
       <c r="H651">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I651">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J651" t="s">
         <v>22</v>
@@ -32634,10 +32654,10 @@
         <v>19</v>
       </c>
       <c r="H652">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I652">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J652" t="s">
         <v>22</v>
@@ -32681,10 +32701,10 @@
         <v>19</v>
       </c>
       <c r="H653">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I653">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J653" t="s">
         <v>22</v>
@@ -32728,10 +32748,10 @@
         <v>19</v>
       </c>
       <c r="H654">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I654">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J654" t="s">
         <v>22</v>
@@ -32775,10 +32795,10 @@
         <v>19</v>
       </c>
       <c r="H655">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I655">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J655" t="s">
         <v>22</v>
@@ -32822,10 +32842,10 @@
         <v>19</v>
       </c>
       <c r="H656">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I656">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J656" t="s">
         <v>22</v>
@@ -32869,10 +32889,10 @@
         <v>19</v>
       </c>
       <c r="H657">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I657">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J657" t="s">
         <v>22</v>
@@ -32916,10 +32936,10 @@
         <v>19</v>
       </c>
       <c r="H658">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I658">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J658" t="s">
         <v>22</v>
@@ -32963,10 +32983,10 @@
         <v>19</v>
       </c>
       <c r="H659">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I659">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J659" t="s">
         <v>22</v>
@@ -33010,10 +33030,10 @@
         <v>19</v>
       </c>
       <c r="H660">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I660">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J660" t="s">
         <v>22</v>
@@ -33057,10 +33077,10 @@
         <v>19</v>
       </c>
       <c r="H661">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I661">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J661" t="s">
         <v>22</v>
@@ -33104,10 +33124,10 @@
         <v>19</v>
       </c>
       <c r="H662">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I662">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J662" t="s">
         <v>22</v>
@@ -33151,10 +33171,10 @@
         <v>19</v>
       </c>
       <c r="H663">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I663">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J663" t="s">
         <v>22</v>
@@ -33198,10 +33218,10 @@
         <v>19</v>
       </c>
       <c r="H664">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I664">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J664" t="s">
         <v>22</v>
@@ -33245,10 +33265,10 @@
         <v>19</v>
       </c>
       <c r="H665">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I665">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J665" t="s">
         <v>22</v>
@@ -33292,10 +33312,10 @@
         <v>19</v>
       </c>
       <c r="H666">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I666">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J666" t="s">
         <v>22</v>
@@ -33339,10 +33359,10 @@
         <v>19</v>
       </c>
       <c r="H667">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I667">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J667" t="s">
         <v>22</v>
@@ -33386,10 +33406,10 @@
         <v>19</v>
       </c>
       <c r="H668">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I668">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J668" t="s">
         <v>22</v>
@@ -33433,10 +33453,10 @@
         <v>19</v>
       </c>
       <c r="H669">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I669">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J669" t="s">
         <v>22</v>
@@ -33480,10 +33500,10 @@
         <v>19</v>
       </c>
       <c r="H670">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I670">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J670" t="s">
         <v>22</v>
@@ -33527,10 +33547,10 @@
         <v>19</v>
       </c>
       <c r="H671">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I671">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J671" t="s">
         <v>22</v>
@@ -33574,10 +33594,10 @@
         <v>19</v>
       </c>
       <c r="H672">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I672">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J672" t="s">
         <v>22</v>
@@ -33621,10 +33641,10 @@
         <v>19</v>
       </c>
       <c r="H673">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I673">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J673" t="s">
         <v>22</v>
@@ -33668,10 +33688,10 @@
         <v>19</v>
       </c>
       <c r="H674">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I674">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J674" t="s">
         <v>22</v>
@@ -33715,10 +33735,10 @@
         <v>19</v>
       </c>
       <c r="H675">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I675">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J675" t="s">
         <v>22</v>
@@ -33762,10 +33782,10 @@
         <v>19</v>
       </c>
       <c r="H676">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I676">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J676" t="s">
         <v>22</v>
@@ -33809,10 +33829,10 @@
         <v>19</v>
       </c>
       <c r="H677">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I677">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J677" t="s">
         <v>22</v>
@@ -33856,10 +33876,10 @@
         <v>19</v>
       </c>
       <c r="H678">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I678">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J678" t="s">
         <v>22</v>
@@ -33903,10 +33923,10 @@
         <v>19</v>
       </c>
       <c r="H679">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I679">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J679" t="s">
         <v>22</v>
@@ -33950,10 +33970,10 @@
         <v>19</v>
       </c>
       <c r="H680">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I680">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J680" t="s">
         <v>22</v>
@@ -33997,10 +34017,10 @@
         <v>19</v>
       </c>
       <c r="H681">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I681">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J681" t="s">
         <v>22</v>
@@ -34044,10 +34064,10 @@
         <v>19</v>
       </c>
       <c r="H682">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I682">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J682" t="s">
         <v>22</v>
@@ -34091,10 +34111,10 @@
         <v>19</v>
       </c>
       <c r="H683">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I683">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J683" t="s">
         <v>22</v>
@@ -34138,10 +34158,10 @@
         <v>19</v>
       </c>
       <c r="H684">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I684">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J684" t="s">
         <v>22</v>
@@ -34185,10 +34205,10 @@
         <v>19</v>
       </c>
       <c r="H685">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I685">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J685" t="s">
         <v>22</v>
@@ -34232,10 +34252,10 @@
         <v>19</v>
       </c>
       <c r="H686">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I686">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J686" t="s">
         <v>22</v>
@@ -34279,10 +34299,10 @@
         <v>19</v>
       </c>
       <c r="H687">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I687">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J687" t="s">
         <v>22</v>
@@ -34326,10 +34346,10 @@
         <v>19</v>
       </c>
       <c r="H688">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I688">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J688" t="s">
         <v>22</v>
@@ -34373,10 +34393,10 @@
         <v>19</v>
       </c>
       <c r="H689">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I689">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J689" t="s">
         <v>22</v>
@@ -34420,10 +34440,10 @@
         <v>19</v>
       </c>
       <c r="H690">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I690">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J690" t="s">
         <v>22</v>
@@ -34467,10 +34487,10 @@
         <v>19</v>
       </c>
       <c r="H691">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I691">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J691" t="s">
         <v>22</v>
@@ -34514,10 +34534,10 @@
         <v>19</v>
       </c>
       <c r="H692">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I692">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J692" t="s">
         <v>22</v>
@@ -34561,10 +34581,10 @@
         <v>19</v>
       </c>
       <c r="H693">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I693">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J693" t="s">
         <v>22</v>
@@ -34608,10 +34628,10 @@
         <v>19</v>
       </c>
       <c r="H694">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I694">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J694" t="s">
         <v>22</v>
@@ -34655,10 +34675,10 @@
         <v>19</v>
       </c>
       <c r="H695">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I695">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J695" t="s">
         <v>22</v>
@@ -34702,10 +34722,10 @@
         <v>19</v>
       </c>
       <c r="H696">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I696">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J696" t="s">
         <v>22</v>
@@ -34749,10 +34769,10 @@
         <v>19</v>
       </c>
       <c r="H697">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I697">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J697" t="s">
         <v>22</v>
@@ -34796,10 +34816,10 @@
         <v>19</v>
       </c>
       <c r="H698">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I698">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J698" t="s">
         <v>22</v>
@@ -34843,10 +34863,10 @@
         <v>19</v>
       </c>
       <c r="H699">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I699">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J699" t="s">
         <v>22</v>
@@ -34890,10 +34910,10 @@
         <v>19</v>
       </c>
       <c r="H700">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I700">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J700" t="s">
         <v>22</v>
@@ -34937,10 +34957,10 @@
         <v>19</v>
       </c>
       <c r="H701">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I701">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J701" t="s">
         <v>22</v>
@@ -34984,10 +35004,10 @@
         <v>19</v>
       </c>
       <c r="H702">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I702">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J702" t="s">
         <v>22</v>
@@ -35010,6 +35030,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Include hybrid in output
</commit_message>
<xml_diff>
--- a/raw/Red book.xlsx
+++ b/raw/Red book.xlsx
@@ -136,8 +136,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -151,11 +153,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P702"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H702"/>
+    <sheetView tabSelected="1" topLeftCell="I679" workbookViewId="0">
+      <selection activeCell="P702" sqref="P509:P702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -26003,6 +26007,9 @@
       <c r="O510">
         <v>2</v>
       </c>
+      <c r="P510">
+        <v>1</v>
+      </c>
     </row>
     <row r="511" spans="1:16" ht="12.75" customHeight="1">
       <c r="A511" s="1">
@@ -26050,6 +26057,9 @@
       <c r="O511">
         <v>2</v>
       </c>
+      <c r="P511">
+        <v>1</v>
+      </c>
     </row>
     <row r="512" spans="1:16" ht="12.75" customHeight="1">
       <c r="A512" s="1">
@@ -26097,8 +26107,11 @@
       <c r="O512">
         <v>2</v>
       </c>
-    </row>
-    <row r="513" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P512">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:16" ht="12.75" customHeight="1">
       <c r="A513" s="1">
         <v>39694</v>
       </c>
@@ -26144,8 +26157,11 @@
       <c r="O513">
         <v>2</v>
       </c>
-    </row>
-    <row r="514" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P513">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" spans="1:16" ht="12.75" customHeight="1">
       <c r="A514" s="1">
         <v>39706</v>
       </c>
@@ -26191,8 +26207,11 @@
       <c r="O514">
         <v>2</v>
       </c>
-    </row>
-    <row r="515" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P514">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:16" ht="12.75" customHeight="1">
       <c r="A515" s="1">
         <v>39721</v>
       </c>
@@ -26238,8 +26257,11 @@
       <c r="O515">
         <v>2</v>
       </c>
-    </row>
-    <row r="516" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P515">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" spans="1:16" ht="12.75" customHeight="1">
       <c r="A516" s="1">
         <v>39735</v>
       </c>
@@ -26285,8 +26307,11 @@
       <c r="O516">
         <v>2</v>
       </c>
-    </row>
-    <row r="517" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P516">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" spans="1:16" ht="12.75" customHeight="1">
       <c r="A517" s="1">
         <v>39750</v>
       </c>
@@ -26332,8 +26357,11 @@
       <c r="O517">
         <v>2</v>
       </c>
-    </row>
-    <row r="518" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P517">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="1:16" ht="12.75" customHeight="1">
       <c r="A518" s="1">
         <v>39769</v>
       </c>
@@ -26379,8 +26407,11 @@
       <c r="O518">
         <v>2</v>
       </c>
-    </row>
-    <row r="519" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P518">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="519" spans="1:16" ht="12.75" customHeight="1">
       <c r="A519" s="1">
         <v>39786</v>
       </c>
@@ -26426,8 +26457,11 @@
       <c r="O519">
         <v>2</v>
       </c>
-    </row>
-    <row r="520" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P519">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="520" spans="1:16" ht="12.75" customHeight="1">
       <c r="A520" s="1">
         <v>39796</v>
       </c>
@@ -26473,8 +26507,11 @@
       <c r="O520">
         <v>2</v>
       </c>
-    </row>
-    <row r="521" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P520">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521" spans="1:16" ht="12.75" customHeight="1">
       <c r="A521" s="1">
         <v>39806</v>
       </c>
@@ -26520,8 +26557,11 @@
       <c r="O521">
         <v>2</v>
       </c>
-    </row>
-    <row r="522" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P521">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" spans="1:16" ht="12.75" customHeight="1">
       <c r="A522" s="1">
         <v>39828</v>
       </c>
@@ -26567,8 +26607,11 @@
       <c r="O522">
         <v>2</v>
       </c>
-    </row>
-    <row r="523" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P522">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" spans="1:16" ht="12.75" customHeight="1">
       <c r="A523" s="1">
         <v>39842</v>
       </c>
@@ -26614,8 +26657,11 @@
       <c r="O523">
         <v>2</v>
       </c>
-    </row>
-    <row r="524" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P523">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" spans="1:16" ht="12.75" customHeight="1">
       <c r="A524" s="1">
         <v>39855</v>
       </c>
@@ -26661,8 +26707,11 @@
       <c r="O524">
         <v>2</v>
       </c>
-    </row>
-    <row r="525" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P524">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525" spans="1:16" ht="12.75" customHeight="1">
       <c r="A525" s="1">
         <v>39869</v>
       </c>
@@ -26708,8 +26757,11 @@
       <c r="O525">
         <v>2</v>
       </c>
-    </row>
-    <row r="526" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P525">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="526" spans="1:16" ht="12.75" customHeight="1">
       <c r="A526" s="1">
         <v>39872</v>
       </c>
@@ -26755,8 +26807,11 @@
       <c r="O526">
         <v>2</v>
       </c>
-    </row>
-    <row r="527" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P526">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527" spans="1:16" ht="12.75" customHeight="1">
       <c r="A527" s="1">
         <v>39884</v>
       </c>
@@ -26802,8 +26857,11 @@
       <c r="O527">
         <v>2</v>
       </c>
-    </row>
-    <row r="528" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P527">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" spans="1:16" ht="12.75" customHeight="1">
       <c r="A528" s="1">
         <v>39889</v>
       </c>
@@ -26849,8 +26907,11 @@
       <c r="O528">
         <v>2</v>
       </c>
-    </row>
-    <row r="529" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P528">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="1:16" ht="12.75" customHeight="1">
       <c r="A529" s="1">
         <v>39892</v>
       </c>
@@ -26896,8 +26957,11 @@
       <c r="O529">
         <v>2</v>
       </c>
-    </row>
-    <row r="530" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P529">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="530" spans="1:16" ht="12.75" customHeight="1">
       <c r="A530" s="1">
         <v>39901</v>
       </c>
@@ -26943,8 +27007,11 @@
       <c r="O530">
         <v>2</v>
       </c>
-    </row>
-    <row r="531" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P530">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="531" spans="1:16" ht="12.75" customHeight="1">
       <c r="A531" s="1">
         <v>39913</v>
       </c>
@@ -26990,8 +27057,11 @@
       <c r="O531">
         <v>2</v>
       </c>
-    </row>
-    <row r="532" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P531">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532" spans="1:16" ht="12.75" customHeight="1">
       <c r="A532" s="1">
         <v>39914</v>
       </c>
@@ -27037,8 +27107,11 @@
       <c r="O532">
         <v>2</v>
       </c>
-    </row>
-    <row r="533" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P532">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="533" spans="1:16" ht="12.75" customHeight="1">
       <c r="A533" s="1">
         <v>39926</v>
       </c>
@@ -27084,8 +27157,11 @@
       <c r="O533">
         <v>2</v>
       </c>
-    </row>
-    <row r="534" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P533">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="534" spans="1:16" ht="12.75" customHeight="1">
       <c r="A534" s="1">
         <v>39928</v>
       </c>
@@ -27131,8 +27207,11 @@
       <c r="O534">
         <v>2</v>
       </c>
-    </row>
-    <row r="535" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P534">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535" spans="1:16" ht="12.75" customHeight="1">
       <c r="A535" s="1">
         <v>39938</v>
       </c>
@@ -27178,8 +27257,11 @@
       <c r="O535">
         <v>2</v>
       </c>
-    </row>
-    <row r="536" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P535">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="536" spans="1:16" ht="12.75" customHeight="1">
       <c r="A536" s="1">
         <v>39952</v>
       </c>
@@ -27225,8 +27307,11 @@
       <c r="O536">
         <v>2</v>
       </c>
-    </row>
-    <row r="537" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P536">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="537" spans="1:16" ht="12.75" customHeight="1">
       <c r="A537" s="1">
         <v>39961</v>
       </c>
@@ -27272,8 +27357,11 @@
       <c r="O537">
         <v>2</v>
       </c>
-    </row>
-    <row r="538" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P537">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="538" spans="1:16" ht="12.75" customHeight="1">
       <c r="A538" s="1">
         <v>39969</v>
       </c>
@@ -27319,8 +27407,11 @@
       <c r="O538">
         <v>2</v>
       </c>
-    </row>
-    <row r="539" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P538">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="539" spans="1:16" ht="12.75" customHeight="1">
       <c r="A539" s="1">
         <v>39977</v>
       </c>
@@ -27366,8 +27457,11 @@
       <c r="O539">
         <v>2</v>
       </c>
-    </row>
-    <row r="540" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P539">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="540" spans="1:16" ht="12.75" customHeight="1">
       <c r="A540" s="1">
         <v>39993</v>
       </c>
@@ -27413,8 +27507,11 @@
       <c r="O540">
         <v>2</v>
       </c>
-    </row>
-    <row r="541" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P540">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" spans="1:16" ht="12.75" customHeight="1">
       <c r="A541" s="1">
         <v>40010</v>
       </c>
@@ -27460,8 +27557,11 @@
       <c r="O541">
         <v>2</v>
       </c>
-    </row>
-    <row r="542" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P541">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="542" spans="1:16" ht="12.75" customHeight="1">
       <c r="A542" s="1">
         <v>40019</v>
       </c>
@@ -27507,8 +27607,11 @@
       <c r="O542">
         <v>2</v>
       </c>
-    </row>
-    <row r="543" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P542">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="543" spans="1:16" ht="12.75" customHeight="1">
       <c r="A543" s="1">
         <v>40022</v>
       </c>
@@ -27554,8 +27657,11 @@
       <c r="O543">
         <v>2</v>
       </c>
-    </row>
-    <row r="544" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P543">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544" spans="1:16" ht="12.75" customHeight="1">
       <c r="A544" s="1">
         <v>40032</v>
       </c>
@@ -27601,8 +27707,11 @@
       <c r="O544">
         <v>2</v>
       </c>
-    </row>
-    <row r="545" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P544">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="545" spans="1:16" ht="12.75" customHeight="1">
       <c r="A545" s="1">
         <v>40032</v>
       </c>
@@ -27648,8 +27757,11 @@
       <c r="O545">
         <v>2</v>
       </c>
-    </row>
-    <row r="546" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P545">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="546" spans="1:16" ht="12.75" customHeight="1">
       <c r="A546" s="1">
         <v>40033</v>
       </c>
@@ -27695,8 +27807,11 @@
       <c r="O546">
         <v>2</v>
       </c>
-    </row>
-    <row r="547" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P546">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="547" spans="1:16" ht="12.75" customHeight="1">
       <c r="A547" s="1">
         <v>40035</v>
       </c>
@@ -27742,8 +27857,11 @@
       <c r="O547">
         <v>2</v>
       </c>
-    </row>
-    <row r="548" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P547">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="548" spans="1:16" ht="12.75" customHeight="1">
       <c r="A548" s="1">
         <v>40037</v>
       </c>
@@ -27789,8 +27907,11 @@
       <c r="O548">
         <v>2</v>
       </c>
-    </row>
-    <row r="549" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P548">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="549" spans="1:16" ht="12.75" customHeight="1">
       <c r="A549" s="1">
         <v>40040</v>
       </c>
@@ -27836,8 +27957,11 @@
       <c r="O549">
         <v>2</v>
       </c>
-    </row>
-    <row r="550" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P549">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="550" spans="1:16" ht="12.75" customHeight="1">
       <c r="A550" s="1">
         <v>40041</v>
       </c>
@@ -27883,8 +28007,11 @@
       <c r="O550">
         <v>2</v>
       </c>
-    </row>
-    <row r="551" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P550">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="551" spans="1:16" ht="12.75" customHeight="1">
       <c r="A551" s="1">
         <v>40043</v>
       </c>
@@ -27930,8 +28057,11 @@
       <c r="O551">
         <v>2</v>
       </c>
-    </row>
-    <row r="552" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P551">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="552" spans="1:16" ht="12.75" customHeight="1">
       <c r="A552" s="1">
         <v>40050</v>
       </c>
@@ -27977,8 +28107,11 @@
       <c r="O552">
         <v>2</v>
       </c>
-    </row>
-    <row r="553" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P552">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="553" spans="1:16" ht="12.75" customHeight="1">
       <c r="A553" s="1">
         <v>40066</v>
       </c>
@@ -28024,8 +28157,11 @@
       <c r="O553">
         <v>2</v>
       </c>
-    </row>
-    <row r="554" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P553">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="554" spans="1:16" ht="12.75" customHeight="1">
       <c r="A554" s="1">
         <v>40080</v>
       </c>
@@ -28071,8 +28207,11 @@
       <c r="O554">
         <v>2</v>
       </c>
-    </row>
-    <row r="555" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P554">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="555" spans="1:16" ht="12.75" customHeight="1">
       <c r="A555" s="1">
         <v>40091</v>
       </c>
@@ -28118,8 +28257,11 @@
       <c r="O555">
         <v>2</v>
       </c>
-    </row>
-    <row r="556" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P555">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="556" spans="1:16" ht="12.75" customHeight="1">
       <c r="A556" s="1">
         <v>40106</v>
       </c>
@@ -28165,8 +28307,11 @@
       <c r="O556">
         <v>2</v>
       </c>
-    </row>
-    <row r="557" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P556">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="557" spans="1:16" ht="12.75" customHeight="1">
       <c r="A557" s="1">
         <v>40116</v>
       </c>
@@ -28212,8 +28357,11 @@
       <c r="O557">
         <v>2</v>
       </c>
-    </row>
-    <row r="558" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P557">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="558" spans="1:16" ht="12.75" customHeight="1">
       <c r="A558" s="1">
         <v>40122</v>
       </c>
@@ -28259,8 +28407,11 @@
       <c r="O558">
         <v>2</v>
       </c>
-    </row>
-    <row r="559" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P558">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="559" spans="1:16" ht="12.75" customHeight="1">
       <c r="A559" s="1">
         <v>40129</v>
       </c>
@@ -28306,8 +28457,11 @@
       <c r="O559">
         <v>2</v>
       </c>
-    </row>
-    <row r="560" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P559">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="560" spans="1:16" ht="12.75" customHeight="1">
       <c r="A560" s="1">
         <v>40148</v>
       </c>
@@ -28353,8 +28507,11 @@
       <c r="O560">
         <v>2</v>
       </c>
-    </row>
-    <row r="561" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P560">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="561" spans="1:16" ht="12.75" customHeight="1">
       <c r="A561" s="1">
         <v>40157</v>
       </c>
@@ -28400,8 +28557,11 @@
       <c r="O561">
         <v>2</v>
       </c>
-    </row>
-    <row r="562" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P561">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="562" spans="1:16" ht="12.75" customHeight="1">
       <c r="A562" s="1">
         <v>40170</v>
       </c>
@@ -28447,8 +28607,11 @@
       <c r="O562">
         <v>2</v>
       </c>
-    </row>
-    <row r="563" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P562">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="563" spans="1:16" ht="12.75" customHeight="1">
       <c r="A563" s="1">
         <v>40184</v>
       </c>
@@ -28494,8 +28657,11 @@
       <c r="O563">
         <v>2</v>
       </c>
-    </row>
-    <row r="564" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P563">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="564" spans="1:16" ht="12.75" customHeight="1">
       <c r="A564" s="1">
         <v>40198</v>
       </c>
@@ -28541,8 +28707,11 @@
       <c r="O564">
         <v>2</v>
       </c>
-    </row>
-    <row r="565" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P564">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="565" spans="1:16" ht="12.75" customHeight="1">
       <c r="A565" s="1">
         <v>40213</v>
       </c>
@@ -28588,8 +28757,11 @@
       <c r="O565">
         <v>2</v>
       </c>
-    </row>
-    <row r="566" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P565">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="566" spans="1:16" ht="12.75" customHeight="1">
       <c r="A566" s="1">
         <v>40247</v>
       </c>
@@ -28635,8 +28807,11 @@
       <c r="O566">
         <v>2</v>
       </c>
-    </row>
-    <row r="567" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P566">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="567" spans="1:16" ht="12.75" customHeight="1">
       <c r="A567" s="1">
         <v>40261</v>
       </c>
@@ -28682,8 +28857,11 @@
       <c r="O567">
         <v>2</v>
       </c>
-    </row>
-    <row r="568" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P567">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="568" spans="1:16" ht="12.75" customHeight="1">
       <c r="A568" s="1">
         <v>40268</v>
       </c>
@@ -28729,8 +28907,11 @@
       <c r="O568">
         <v>2</v>
       </c>
-    </row>
-    <row r="569" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P568">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="569" spans="1:16" ht="12.75" customHeight="1">
       <c r="A569" s="1">
         <v>40275</v>
       </c>
@@ -28776,8 +28957,11 @@
       <c r="O569">
         <v>2</v>
       </c>
-    </row>
-    <row r="570" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P569">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="570" spans="1:16" ht="12.75" customHeight="1">
       <c r="A570" s="1">
         <v>40288</v>
       </c>
@@ -28823,8 +29007,11 @@
       <c r="O570">
         <v>2</v>
       </c>
-    </row>
-    <row r="571" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P570">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="571" spans="1:16" ht="12.75" customHeight="1">
       <c r="A571" s="1">
         <v>40308</v>
       </c>
@@ -28870,8 +29057,11 @@
       <c r="O571">
         <v>2</v>
       </c>
-    </row>
-    <row r="572" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P571">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="572" spans="1:16" ht="12.75" customHeight="1">
       <c r="A572" s="1">
         <v>40320</v>
       </c>
@@ -28917,8 +29107,11 @@
       <c r="O572">
         <v>2</v>
       </c>
-    </row>
-    <row r="573" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P572">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="573" spans="1:16" ht="12.75" customHeight="1">
       <c r="A573" s="1">
         <v>40334</v>
       </c>
@@ -28964,8 +29157,11 @@
       <c r="O573">
         <v>2</v>
       </c>
-    </row>
-    <row r="574" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P573">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="574" spans="1:16" ht="12.75" customHeight="1">
       <c r="A574" s="1">
         <v>40346</v>
       </c>
@@ -29011,8 +29207,11 @@
       <c r="O574">
         <v>2</v>
       </c>
-    </row>
-    <row r="575" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P574">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="575" spans="1:16" ht="12.75" customHeight="1">
       <c r="A575" s="1">
         <v>40350</v>
       </c>
@@ -29058,8 +29257,11 @@
       <c r="O575">
         <v>2</v>
       </c>
-    </row>
-    <row r="576" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P575">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="576" spans="1:16" ht="12.75" customHeight="1">
       <c r="A576" s="1">
         <v>40365</v>
       </c>
@@ -29105,8 +29307,11 @@
       <c r="O576">
         <v>2</v>
       </c>
-    </row>
-    <row r="577" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P576">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="577" spans="1:16" ht="12.75" customHeight="1">
       <c r="A577" s="1">
         <v>40380</v>
       </c>
@@ -29152,8 +29357,11 @@
       <c r="O577">
         <v>2</v>
       </c>
-    </row>
-    <row r="578" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P577">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="578" spans="1:16" ht="12.75" customHeight="1">
       <c r="A578" s="1">
         <v>40396</v>
       </c>
@@ -29199,8 +29407,11 @@
       <c r="O578">
         <v>2</v>
       </c>
-    </row>
-    <row r="579" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P578">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="579" spans="1:16" ht="12.75" customHeight="1">
       <c r="A579" s="1">
         <v>40404</v>
       </c>
@@ -29246,8 +29457,11 @@
       <c r="O579">
         <v>2</v>
       </c>
-    </row>
-    <row r="580" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P579">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="580" spans="1:16" ht="12.75" customHeight="1">
       <c r="A580" s="1">
         <v>40406</v>
       </c>
@@ -29293,8 +29507,11 @@
       <c r="O580">
         <v>2</v>
       </c>
-    </row>
-    <row r="581" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P580">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="581" spans="1:16" ht="12.75" customHeight="1">
       <c r="A581" s="1">
         <v>40411</v>
       </c>
@@ -29340,8 +29557,11 @@
       <c r="O581">
         <v>2</v>
       </c>
-    </row>
-    <row r="582" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P581">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="582" spans="1:16" ht="12.75" customHeight="1">
       <c r="A582" s="1">
         <v>40421</v>
       </c>
@@ -29387,8 +29607,11 @@
       <c r="O582">
         <v>2</v>
       </c>
-    </row>
-    <row r="583" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P582">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="583" spans="1:16" ht="12.75" customHeight="1">
       <c r="A583" s="1">
         <v>40437</v>
       </c>
@@ -29434,8 +29657,11 @@
       <c r="O583">
         <v>2</v>
       </c>
-    </row>
-    <row r="584" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P583">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="584" spans="1:16" ht="12.75" customHeight="1">
       <c r="A584" s="1">
         <v>40442</v>
       </c>
@@ -29481,8 +29707,11 @@
       <c r="O584">
         <v>2</v>
       </c>
-    </row>
-    <row r="585" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P584">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="585" spans="1:16" ht="12.75" customHeight="1">
       <c r="A585" s="1">
         <v>40451</v>
       </c>
@@ -29528,8 +29757,11 @@
       <c r="O585">
         <v>2</v>
       </c>
-    </row>
-    <row r="586" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P585">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="586" spans="1:16" ht="12.75" customHeight="1">
       <c r="A586" s="1">
         <v>40462</v>
       </c>
@@ -29575,8 +29807,11 @@
       <c r="O586">
         <v>2</v>
       </c>
-    </row>
-    <row r="587" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P586">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="587" spans="1:16" ht="12.75" customHeight="1">
       <c r="A587" s="1">
         <v>40473</v>
       </c>
@@ -29622,8 +29857,11 @@
       <c r="O587">
         <v>2</v>
       </c>
-    </row>
-    <row r="588" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P587">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="588" spans="1:16" ht="12.75" customHeight="1">
       <c r="A588" s="1">
         <v>40486</v>
       </c>
@@ -29669,8 +29907,11 @@
       <c r="O588">
         <v>2</v>
       </c>
-    </row>
-    <row r="589" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P588">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="589" spans="1:16" ht="12.75" customHeight="1">
       <c r="A589" s="1">
         <v>40495</v>
       </c>
@@ -29716,8 +29957,11 @@
       <c r="O589">
         <v>2</v>
       </c>
-    </row>
-    <row r="590" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P589">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="590" spans="1:16" ht="12.75" customHeight="1">
       <c r="A590" s="1">
         <v>40505</v>
       </c>
@@ -29763,8 +30007,11 @@
       <c r="O590">
         <v>2</v>
       </c>
-    </row>
-    <row r="591" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P590">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="591" spans="1:16" ht="12.75" customHeight="1">
       <c r="A591" s="1">
         <v>40511</v>
       </c>
@@ -29810,8 +30057,11 @@
       <c r="O591">
         <v>2</v>
       </c>
-    </row>
-    <row r="592" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P591">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="592" spans="1:16" ht="12.75" customHeight="1">
       <c r="A592" s="1">
         <v>40525</v>
       </c>
@@ -29857,8 +30107,11 @@
       <c r="O592">
         <v>2</v>
       </c>
-    </row>
-    <row r="593" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P592">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="593" spans="1:16" ht="12.75" customHeight="1">
       <c r="A593" s="1">
         <v>40535</v>
       </c>
@@ -29904,8 +30157,11 @@
       <c r="O593">
         <v>2</v>
       </c>
-    </row>
-    <row r="594" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P593">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="594" spans="1:16" ht="12.75" customHeight="1">
       <c r="A594" s="1">
         <v>40551</v>
       </c>
@@ -29951,8 +30207,11 @@
       <c r="O594">
         <v>2</v>
       </c>
-    </row>
-    <row r="595" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P594">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="595" spans="1:16" ht="12.75" customHeight="1">
       <c r="A595" s="1">
         <v>40563</v>
       </c>
@@ -29998,8 +30257,11 @@
       <c r="O595">
         <v>2</v>
       </c>
-    </row>
-    <row r="596" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P595">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="596" spans="1:16" ht="12.75" customHeight="1">
       <c r="A596" s="1">
         <v>40571</v>
       </c>
@@ -30045,8 +30307,11 @@
       <c r="O596">
         <v>2</v>
       </c>
-    </row>
-    <row r="597" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P596">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="597" spans="1:16" ht="12.75" customHeight="1">
       <c r="A597" s="1">
         <v>40584</v>
       </c>
@@ -30092,8 +30357,11 @@
       <c r="O597">
         <v>2</v>
       </c>
-    </row>
-    <row r="598" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P597">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="598" spans="1:16" ht="12.75" customHeight="1">
       <c r="A598" s="1">
         <v>40600</v>
       </c>
@@ -30139,8 +30407,11 @@
       <c r="O598">
         <v>2</v>
       </c>
-    </row>
-    <row r="599" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P598">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="599" spans="1:16" ht="12.75" customHeight="1">
       <c r="A599" s="1">
         <v>40609</v>
       </c>
@@ -30186,8 +30457,11 @@
       <c r="O599">
         <v>2</v>
       </c>
-    </row>
-    <row r="600" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P599">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="600" spans="1:16" ht="12.75" customHeight="1">
       <c r="A600" s="1">
         <v>40619</v>
       </c>
@@ -30233,8 +30507,11 @@
       <c r="O600">
         <v>2</v>
       </c>
-    </row>
-    <row r="601" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P600">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="601" spans="1:16" ht="12.75" customHeight="1">
       <c r="A601" s="1">
         <v>40625</v>
       </c>
@@ -30280,8 +30557,11 @@
       <c r="O601">
         <v>2</v>
       </c>
-    </row>
-    <row r="602" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P601">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="602" spans="1:16" ht="12.75" customHeight="1">
       <c r="A602" s="1">
         <v>40637</v>
       </c>
@@ -30327,8 +30607,11 @@
       <c r="O602">
         <v>2</v>
       </c>
-    </row>
-    <row r="603" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P602">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="603" spans="1:16" ht="12.75" customHeight="1">
       <c r="A603" s="1">
         <v>40647</v>
       </c>
@@ -30374,8 +30657,11 @@
       <c r="O603">
         <v>2</v>
       </c>
-    </row>
-    <row r="604" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P603">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="604" spans="1:16" ht="12.75" customHeight="1">
       <c r="A604" s="1">
         <v>40650</v>
       </c>
@@ -30421,8 +30707,11 @@
       <c r="O604">
         <v>2</v>
       </c>
-    </row>
-    <row r="605" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P604">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="605" spans="1:16" ht="12.75" customHeight="1">
       <c r="A605" s="1">
         <v>40650</v>
       </c>
@@ -30468,8 +30757,11 @@
       <c r="O605">
         <v>2</v>
       </c>
-    </row>
-    <row r="606" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P605">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="606" spans="1:16" ht="12.75" customHeight="1">
       <c r="A606" s="1">
         <v>40656</v>
       </c>
@@ -30515,8 +30807,11 @@
       <c r="O606">
         <v>2</v>
       </c>
-    </row>
-    <row r="607" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P606">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="607" spans="1:16" ht="12.75" customHeight="1">
       <c r="A607" s="1">
         <v>40668</v>
       </c>
@@ -30562,8 +30857,11 @@
       <c r="O607">
         <v>2</v>
       </c>
-    </row>
-    <row r="608" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P607">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="608" spans="1:16" ht="12.75" customHeight="1">
       <c r="A608" s="1">
         <v>40675</v>
       </c>
@@ -30609,8 +30907,11 @@
       <c r="O608">
         <v>2</v>
       </c>
-    </row>
-    <row r="609" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P608">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="609" spans="1:16" ht="12.75" customHeight="1">
       <c r="A609" s="1">
         <v>40686</v>
       </c>
@@ -30656,8 +30957,11 @@
       <c r="O609">
         <v>2</v>
       </c>
-    </row>
-    <row r="610" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P609">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="610" spans="1:16" ht="12.75" customHeight="1">
       <c r="A610" s="1">
         <v>40695</v>
       </c>
@@ -30703,8 +31007,11 @@
       <c r="O610">
         <v>2</v>
       </c>
-    </row>
-    <row r="611" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P610">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="611" spans="1:16" ht="12.75" customHeight="1">
       <c r="A611" s="1">
         <v>40707</v>
       </c>
@@ -30750,8 +31057,11 @@
       <c r="O611">
         <v>2</v>
       </c>
-    </row>
-    <row r="612" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P611">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="612" spans="1:16" ht="12.75" customHeight="1">
       <c r="A612" s="1">
         <v>40723</v>
       </c>
@@ -30797,8 +31107,11 @@
       <c r="O612">
         <v>2</v>
       </c>
-    </row>
-    <row r="613" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P612">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="613" spans="1:16" ht="12.75" customHeight="1">
       <c r="A613" s="1">
         <v>40737</v>
       </c>
@@ -30844,8 +31157,11 @@
       <c r="O613">
         <v>2</v>
       </c>
-    </row>
-    <row r="614" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P613">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="614" spans="1:16" ht="12.75" customHeight="1">
       <c r="A614" s="1">
         <v>40741</v>
       </c>
@@ -30891,8 +31207,11 @@
       <c r="O614">
         <v>2</v>
       </c>
-    </row>
-    <row r="615" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P614">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="615" spans="1:16" ht="12.75" customHeight="1">
       <c r="A615" s="1">
         <v>40752</v>
       </c>
@@ -30938,8 +31257,11 @@
       <c r="O615">
         <v>2</v>
       </c>
-    </row>
-    <row r="616" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P615">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="616" spans="1:16" ht="12.75" customHeight="1">
       <c r="A616" s="1">
         <v>40761</v>
       </c>
@@ -30985,8 +31307,11 @@
       <c r="O616">
         <v>2</v>
       </c>
-    </row>
-    <row r="617" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P616">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="617" spans="1:16" ht="12.75" customHeight="1">
       <c r="A617" s="1">
         <v>40762</v>
       </c>
@@ -31032,8 +31357,11 @@
       <c r="O617">
         <v>2</v>
       </c>
-    </row>
-    <row r="618" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P617">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="618" spans="1:16" ht="12.75" customHeight="1">
       <c r="A618" s="1">
         <v>40767</v>
       </c>
@@ -31079,8 +31407,11 @@
       <c r="O618">
         <v>2</v>
       </c>
-    </row>
-    <row r="619" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P618">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="619" spans="1:16" ht="12.75" customHeight="1">
       <c r="A619" s="1">
         <v>40771</v>
       </c>
@@ -31126,8 +31457,11 @@
       <c r="O619">
         <v>2</v>
       </c>
-    </row>
-    <row r="620" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P619">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="620" spans="1:16" ht="12.75" customHeight="1">
       <c r="A620" s="1">
         <v>40782</v>
       </c>
@@ -31173,8 +31507,11 @@
       <c r="O620">
         <v>2</v>
       </c>
-    </row>
-    <row r="621" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P620">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="621" spans="1:16" ht="12.75" customHeight="1">
       <c r="A621" s="1">
         <v>40789</v>
       </c>
@@ -31220,8 +31557,11 @@
       <c r="O621">
         <v>2</v>
       </c>
-    </row>
-    <row r="622" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P621">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="622" spans="1:16" ht="12.75" customHeight="1">
       <c r="A622" s="1">
         <v>40795</v>
       </c>
@@ -31267,8 +31607,11 @@
       <c r="O622">
         <v>2</v>
       </c>
-    </row>
-    <row r="623" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P622">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="623" spans="1:16" ht="12.75" customHeight="1">
       <c r="A623" s="1">
         <v>40795</v>
       </c>
@@ -31314,8 +31657,11 @@
       <c r="O623">
         <v>2</v>
       </c>
-    </row>
-    <row r="624" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P623">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="624" spans="1:16" ht="12.75" customHeight="1">
       <c r="A624" s="1">
         <v>40823</v>
       </c>
@@ -31361,8 +31707,11 @@
       <c r="O624">
         <v>2</v>
       </c>
-    </row>
-    <row r="625" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P624">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="625" spans="1:16" ht="12.75" customHeight="1">
       <c r="A625" s="1">
         <v>40833</v>
       </c>
@@ -31408,8 +31757,11 @@
       <c r="O625">
         <v>2</v>
       </c>
-    </row>
-    <row r="626" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P625">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="626" spans="1:16" ht="12.75" customHeight="1">
       <c r="A626" s="1">
         <v>40837</v>
       </c>
@@ -31455,8 +31807,11 @@
       <c r="O626">
         <v>2</v>
       </c>
-    </row>
-    <row r="627" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P626">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="627" spans="1:16" ht="12.75" customHeight="1">
       <c r="A627" s="1">
         <v>40838</v>
       </c>
@@ -31502,8 +31857,11 @@
       <c r="O627">
         <v>2</v>
       </c>
-    </row>
-    <row r="628" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P627">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="628" spans="1:16" ht="12.75" customHeight="1">
       <c r="A628" s="1">
         <v>40840</v>
       </c>
@@ -31549,8 +31907,11 @@
       <c r="O628">
         <v>2</v>
       </c>
-    </row>
-    <row r="629" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P628">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="629" spans="1:16" ht="12.75" customHeight="1">
       <c r="A629" s="1">
         <v>40841</v>
       </c>
@@ -31596,8 +31957,11 @@
       <c r="O629">
         <v>2</v>
       </c>
-    </row>
-    <row r="630" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P629">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="630" spans="1:16" ht="12.75" customHeight="1">
       <c r="A630" s="1">
         <v>40850</v>
       </c>
@@ -31643,8 +32007,11 @@
       <c r="O630">
         <v>2</v>
       </c>
-    </row>
-    <row r="631" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P630">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="631" spans="1:16" ht="12.75" customHeight="1">
       <c r="A631" s="1">
         <v>40853</v>
       </c>
@@ -31690,8 +32057,11 @@
       <c r="O631">
         <v>2</v>
       </c>
-    </row>
-    <row r="632" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P631">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="632" spans="1:16" ht="12.75" customHeight="1">
       <c r="A632" s="1">
         <v>40853</v>
       </c>
@@ -31737,8 +32107,11 @@
       <c r="O632">
         <v>2</v>
       </c>
-    </row>
-    <row r="633" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P632">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="633" spans="1:16" ht="12.75" customHeight="1">
       <c r="A633" s="1">
         <v>40867</v>
       </c>
@@ -31784,8 +32157,11 @@
       <c r="O633">
         <v>2</v>
       </c>
-    </row>
-    <row r="634" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P633">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="634" spans="1:16" ht="12.75" customHeight="1">
       <c r="A634" s="1">
         <v>40879</v>
       </c>
@@ -31831,8 +32207,11 @@
       <c r="O634">
         <v>2</v>
       </c>
-    </row>
-    <row r="635" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P634">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="635" spans="1:16" ht="12.75" customHeight="1">
       <c r="A635" s="1">
         <v>40898</v>
       </c>
@@ -31878,8 +32257,11 @@
       <c r="O635">
         <v>2</v>
       </c>
-    </row>
-    <row r="636" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P635">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="636" spans="1:16" ht="12.75" customHeight="1">
       <c r="A636" s="1">
         <v>40904</v>
       </c>
@@ -31925,8 +32307,11 @@
       <c r="O636">
         <v>2</v>
       </c>
-    </row>
-    <row r="637" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P636">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="637" spans="1:16" ht="12.75" customHeight="1">
       <c r="A637" s="1">
         <v>40915</v>
       </c>
@@ -31972,8 +32357,11 @@
       <c r="O637">
         <v>2</v>
       </c>
-    </row>
-    <row r="638" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P637">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="638" spans="1:16" ht="12.75" customHeight="1">
       <c r="A638" s="1">
         <v>40923</v>
       </c>
@@ -32019,8 +32407,11 @@
       <c r="O638">
         <v>2</v>
       </c>
-    </row>
-    <row r="639" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P638">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="639" spans="1:16" ht="12.75" customHeight="1">
       <c r="A639" s="1">
         <v>40936</v>
       </c>
@@ -32066,8 +32457,11 @@
       <c r="O639">
         <v>2</v>
       </c>
-    </row>
-    <row r="640" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P639">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="640" spans="1:16" ht="12.75" customHeight="1">
       <c r="A640" s="1">
         <v>40948</v>
       </c>
@@ -32113,8 +32507,11 @@
       <c r="O640">
         <v>2</v>
       </c>
-    </row>
-    <row r="641" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P640">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="641" spans="1:16" ht="12.75" customHeight="1">
       <c r="A641" s="1">
         <v>40957</v>
       </c>
@@ -32160,8 +32557,11 @@
       <c r="O641">
         <v>2</v>
       </c>
-    </row>
-    <row r="642" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P641">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="642" spans="1:16" ht="12.75" customHeight="1">
       <c r="A642" s="1">
         <v>40976</v>
       </c>
@@ -32207,8 +32607,11 @@
       <c r="O642">
         <v>2</v>
       </c>
-    </row>
-    <row r="643" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P642">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="643" spans="1:16" ht="12.75" customHeight="1">
       <c r="A643" s="1">
         <v>40990</v>
       </c>
@@ -32254,8 +32657,11 @@
       <c r="O643">
         <v>2</v>
       </c>
-    </row>
-    <row r="644" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P643">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="644" spans="1:16" ht="12.75" customHeight="1">
       <c r="A644" s="1">
         <v>40993</v>
       </c>
@@ -32301,8 +32707,11 @@
       <c r="O644">
         <v>2</v>
       </c>
-    </row>
-    <row r="645" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P644">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="645" spans="1:16" ht="12.75" customHeight="1">
       <c r="A645" s="1">
         <v>40998</v>
       </c>
@@ -32348,8 +32757,11 @@
       <c r="O645">
         <v>2</v>
       </c>
-    </row>
-    <row r="646" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P645">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="646" spans="1:16" ht="12.75" customHeight="1">
       <c r="A646" s="1">
         <v>41011</v>
       </c>
@@ -32395,8 +32807,11 @@
       <c r="O646">
         <v>2</v>
       </c>
-    </row>
-    <row r="647" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P646">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="647" spans="1:16" ht="12.75" customHeight="1">
       <c r="A647" s="1">
         <v>41027</v>
       </c>
@@ -32442,8 +32857,11 @@
       <c r="O647">
         <v>2</v>
       </c>
-    </row>
-    <row r="648" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P647">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="648" spans="1:16" ht="12.75" customHeight="1">
       <c r="A648" s="1">
         <v>41041</v>
       </c>
@@ -32489,8 +32907,11 @@
       <c r="O648">
         <v>2</v>
       </c>
-    </row>
-    <row r="649" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P648">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="649" spans="1:16" ht="12.75" customHeight="1">
       <c r="A649" s="1">
         <v>41050</v>
       </c>
@@ -32536,8 +32957,11 @@
       <c r="O649">
         <v>2</v>
       </c>
-    </row>
-    <row r="650" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P649">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="650" spans="1:16" ht="12.75" customHeight="1">
       <c r="A650" s="1">
         <v>41061</v>
       </c>
@@ -32583,8 +33007,11 @@
       <c r="O650">
         <v>2</v>
       </c>
-    </row>
-    <row r="651" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P650">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="651" spans="1:16" ht="12.75" customHeight="1">
       <c r="A651" s="1">
         <v>41074</v>
       </c>
@@ -32630,8 +33057,11 @@
       <c r="O651">
         <v>2</v>
       </c>
-    </row>
-    <row r="652" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P651">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="652" spans="1:16" ht="12.75" customHeight="1">
       <c r="A652" s="1">
         <v>41082</v>
       </c>
@@ -32677,8 +33107,11 @@
       <c r="O652">
         <v>2</v>
       </c>
-    </row>
-    <row r="653" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P652">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="653" spans="1:16" ht="12.75" customHeight="1">
       <c r="A653" s="1">
         <v>41094</v>
       </c>
@@ -32724,8 +33157,11 @@
       <c r="O653">
         <v>2</v>
       </c>
-    </row>
-    <row r="654" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P653">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="654" spans="1:16" ht="12.75" customHeight="1">
       <c r="A654" s="1">
         <v>41107</v>
       </c>
@@ -32771,8 +33207,11 @@
       <c r="O654">
         <v>2</v>
       </c>
-    </row>
-    <row r="655" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P654">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="655" spans="1:16" ht="12.75" customHeight="1">
       <c r="A655" s="1">
         <v>41118</v>
       </c>
@@ -32818,8 +33257,11 @@
       <c r="O655">
         <v>2</v>
       </c>
-    </row>
-    <row r="656" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P655">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="656" spans="1:16" ht="12.75" customHeight="1">
       <c r="A656" s="1">
         <v>41125</v>
       </c>
@@ -32865,8 +33307,11 @@
       <c r="O656">
         <v>2</v>
       </c>
-    </row>
-    <row r="657" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P656">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="657" spans="1:16" ht="12.75" customHeight="1">
       <c r="A657" s="1">
         <v>41144</v>
       </c>
@@ -32912,8 +33357,11 @@
       <c r="O657">
         <v>2</v>
       </c>
-    </row>
-    <row r="658" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P657">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="658" spans="1:16" ht="12.75" customHeight="1">
       <c r="A658" s="1">
         <v>41146</v>
       </c>
@@ -32959,8 +33407,11 @@
       <c r="O658">
         <v>2</v>
       </c>
-    </row>
-    <row r="659" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P658">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="659" spans="1:16" ht="12.75" customHeight="1">
       <c r="A659" s="1">
         <v>41164</v>
       </c>
@@ -33006,8 +33457,11 @@
       <c r="O659">
         <v>2</v>
       </c>
-    </row>
-    <row r="660" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P659">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="660" spans="1:16" ht="12.75" customHeight="1">
       <c r="A660" s="1">
         <v>41172</v>
       </c>
@@ -33053,8 +33507,11 @@
       <c r="O660">
         <v>2</v>
       </c>
-    </row>
-    <row r="661" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P660">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="661" spans="1:16" ht="12.75" customHeight="1">
       <c r="A661" s="1">
         <v>41176</v>
       </c>
@@ -33100,8 +33557,11 @@
       <c r="O661">
         <v>2</v>
       </c>
-    </row>
-    <row r="662" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P661">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="662" spans="1:16" ht="12.75" customHeight="1">
       <c r="A662" s="1">
         <v>41180</v>
       </c>
@@ -33147,8 +33607,11 @@
       <c r="O662">
         <v>2</v>
       </c>
-    </row>
-    <row r="663" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P662">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="663" spans="1:16" ht="12.75" customHeight="1">
       <c r="A663" s="1">
         <v>41184</v>
       </c>
@@ -33194,8 +33657,11 @@
       <c r="O663">
         <v>2</v>
       </c>
-    </row>
-    <row r="664" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P663">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="664" spans="1:16" ht="12.75" customHeight="1">
       <c r="A664" s="1">
         <v>41204</v>
       </c>
@@ -33241,8 +33707,11 @@
       <c r="O664">
         <v>2</v>
       </c>
-    </row>
-    <row r="665" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P664">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="665" spans="1:16" ht="12.75" customHeight="1">
       <c r="A665" s="1">
         <v>41219</v>
       </c>
@@ -33288,8 +33757,11 @@
       <c r="O665">
         <v>2</v>
       </c>
-    </row>
-    <row r="666" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P665">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="666" spans="1:16" ht="12.75" customHeight="1">
       <c r="A666" s="1">
         <v>41234</v>
       </c>
@@ -33335,8 +33807,11 @@
       <c r="O666">
         <v>2</v>
       </c>
-    </row>
-    <row r="667" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P666">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="667" spans="1:16" ht="12.75" customHeight="1">
       <c r="A667" s="1">
         <v>41250</v>
       </c>
@@ -33382,8 +33857,11 @@
       <c r="O667">
         <v>2</v>
       </c>
-    </row>
-    <row r="668" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P667">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="668" spans="1:16" ht="12.75" customHeight="1">
       <c r="A668" s="1">
         <v>41263</v>
       </c>
@@ -33429,8 +33907,11 @@
       <c r="O668">
         <v>2</v>
       </c>
-    </row>
-    <row r="669" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P668">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="669" spans="1:16" ht="12.75" customHeight="1">
       <c r="A669" s="1">
         <v>41270</v>
       </c>
@@ -33476,8 +33957,11 @@
       <c r="O669">
         <v>2</v>
       </c>
-    </row>
-    <row r="670" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P669">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="670" spans="1:16" ht="12.75" customHeight="1">
       <c r="A670" s="1">
         <v>41282</v>
       </c>
@@ -33523,8 +34007,11 @@
       <c r="O670">
         <v>2</v>
       </c>
-    </row>
-    <row r="671" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P670">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="671" spans="1:16" ht="12.75" customHeight="1">
       <c r="A671" s="1">
         <v>41293</v>
       </c>
@@ -33570,8 +34057,11 @@
       <c r="O671">
         <v>2</v>
       </c>
-    </row>
-    <row r="672" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P671">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="672" spans="1:16" ht="12.75" customHeight="1">
       <c r="A672" s="1">
         <v>41304</v>
       </c>
@@ -33617,8 +34107,11 @@
       <c r="O672">
         <v>2</v>
       </c>
-    </row>
-    <row r="673" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P672">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="673" spans="1:16" ht="12.75" customHeight="1">
       <c r="A673" s="1">
         <v>41319</v>
       </c>
@@ -33664,8 +34157,11 @@
       <c r="O673">
         <v>2</v>
       </c>
-    </row>
-    <row r="674" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P673">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="674" spans="1:16" ht="12.75" customHeight="1">
       <c r="A674" s="1">
         <v>41333</v>
       </c>
@@ -33711,8 +34207,11 @@
       <c r="O674">
         <v>2</v>
       </c>
-    </row>
-    <row r="675" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P674">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="675" spans="1:16" ht="12.75" customHeight="1">
       <c r="A675" s="1">
         <v>41348</v>
       </c>
@@ -33758,8 +34257,11 @@
       <c r="O675">
         <v>2</v>
       </c>
-    </row>
-    <row r="676" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P675">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="676" spans="1:16" ht="12.75" customHeight="1">
       <c r="A676" s="1">
         <v>41353</v>
       </c>
@@ -33805,8 +34307,11 @@
       <c r="O676">
         <v>2</v>
       </c>
-    </row>
-    <row r="677" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P676">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="677" spans="1:16" ht="12.75" customHeight="1">
       <c r="A677" s="1">
         <v>41356</v>
       </c>
@@ -33852,8 +34357,11 @@
       <c r="O677">
         <v>2</v>
       </c>
-    </row>
-    <row r="678" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P677">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="678" spans="1:16" ht="12.75" customHeight="1">
       <c r="A678" s="1">
         <v>41363</v>
       </c>
@@ -33899,8 +34407,11 @@
       <c r="O678">
         <v>2</v>
       </c>
-    </row>
-    <row r="679" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P678">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="679" spans="1:16" ht="12.75" customHeight="1">
       <c r="A679" s="1">
         <v>41370</v>
       </c>
@@ -33946,8 +34457,11 @@
       <c r="O679">
         <v>2</v>
       </c>
-    </row>
-    <row r="680" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P679">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="680" spans="1:16" ht="12.75" customHeight="1">
       <c r="A680" s="1">
         <v>41382</v>
       </c>
@@ -33993,8 +34507,11 @@
       <c r="O680">
         <v>2</v>
       </c>
-    </row>
-    <row r="681" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P680">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="681" spans="1:16" ht="12.75" customHeight="1">
       <c r="A681" s="1">
         <v>41389</v>
       </c>
@@ -34040,8 +34557,11 @@
       <c r="O681">
         <v>2</v>
       </c>
-    </row>
-    <row r="682" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P681">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="682" spans="1:16" ht="12.75" customHeight="1">
       <c r="A682" s="1">
         <v>41401</v>
       </c>
@@ -34087,8 +34607,11 @@
       <c r="O682">
         <v>2</v>
       </c>
-    </row>
-    <row r="683" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P682">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="683" spans="1:16" ht="12.75" customHeight="1">
       <c r="A683" s="1">
         <v>41409</v>
       </c>
@@ -34134,8 +34657,11 @@
       <c r="O683">
         <v>2</v>
       </c>
-    </row>
-    <row r="684" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P683">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="684" spans="1:16" ht="12.75" customHeight="1">
       <c r="A684" s="1">
         <v>41416</v>
       </c>
@@ -34181,8 +34707,11 @@
       <c r="O684">
         <v>2</v>
       </c>
-    </row>
-    <row r="685" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P684">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="685" spans="1:16" ht="12.75" customHeight="1">
       <c r="A685" s="1">
         <v>41427</v>
       </c>
@@ -34228,8 +34757,11 @@
       <c r="O685">
         <v>2</v>
       </c>
-    </row>
-    <row r="686" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P685">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="686" spans="1:16" ht="12.75" customHeight="1">
       <c r="A686" s="1">
         <v>41442</v>
       </c>
@@ -34275,8 +34807,11 @@
       <c r="O686">
         <v>2</v>
       </c>
-    </row>
-    <row r="687" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P686">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="687" spans="1:16" ht="12.75" customHeight="1">
       <c r="A687" s="1">
         <v>41460</v>
       </c>
@@ -34322,8 +34857,11 @@
       <c r="O687">
         <v>2</v>
       </c>
-    </row>
-    <row r="688" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P687">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="688" spans="1:16" ht="12.75" customHeight="1">
       <c r="A688" s="1">
         <v>41461</v>
       </c>
@@ -34369,8 +34907,11 @@
       <c r="O688">
         <v>2</v>
       </c>
-    </row>
-    <row r="689" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P688">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="689" spans="1:16" ht="12.75" customHeight="1">
       <c r="A689" s="1">
         <v>41477</v>
       </c>
@@ -34416,8 +34957,11 @@
       <c r="O689">
         <v>2</v>
       </c>
-    </row>
-    <row r="690" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P689">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="690" spans="1:16" ht="12.75" customHeight="1">
       <c r="A690" s="1">
         <v>41482</v>
       </c>
@@ -34463,8 +35007,11 @@
       <c r="O690">
         <v>2</v>
       </c>
-    </row>
-    <row r="691" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P690">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="691" spans="1:16" ht="12.75" customHeight="1">
       <c r="A691" s="1">
         <v>41489</v>
       </c>
@@ -34510,8 +35057,11 @@
       <c r="O691">
         <v>2</v>
       </c>
-    </row>
-    <row r="692" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P691">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="692" spans="1:16" ht="12.75" customHeight="1">
       <c r="A692" s="1">
         <v>41491</v>
       </c>
@@ -34557,8 +35107,11 @@
       <c r="O692">
         <v>2</v>
       </c>
-    </row>
-    <row r="693" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P692">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="693" spans="1:16" ht="12.75" customHeight="1">
       <c r="A693" s="1">
         <v>41507</v>
       </c>
@@ -34604,8 +35157,11 @@
       <c r="O693">
         <v>2</v>
       </c>
-    </row>
-    <row r="694" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P693">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="694" spans="1:16" ht="12.75" customHeight="1">
       <c r="A694" s="1">
         <v>41524</v>
       </c>
@@ -34651,8 +35207,11 @@
       <c r="O694">
         <v>2</v>
       </c>
-    </row>
-    <row r="695" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P694">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="695" spans="1:16" ht="12.75" customHeight="1">
       <c r="A695" s="1">
         <v>41541</v>
       </c>
@@ -34698,8 +35257,11 @@
       <c r="O695">
         <v>2</v>
       </c>
-    </row>
-    <row r="696" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P695">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="696" spans="1:16" ht="12.75" customHeight="1">
       <c r="A696" s="1">
         <v>41555</v>
       </c>
@@ -34745,8 +35307,11 @@
       <c r="O696">
         <v>2</v>
       </c>
-    </row>
-    <row r="697" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P696">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="697" spans="1:16" ht="12.75" customHeight="1">
       <c r="A697" s="1">
         <v>41570</v>
       </c>
@@ -34792,8 +35357,11 @@
       <c r="O697">
         <v>2</v>
       </c>
-    </row>
-    <row r="698" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P697">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="698" spans="1:16" ht="12.75" customHeight="1">
       <c r="A698" s="1">
         <v>41585</v>
       </c>
@@ -34839,8 +35407,11 @@
       <c r="O698">
         <v>2</v>
       </c>
-    </row>
-    <row r="699" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P698">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="699" spans="1:16" ht="12.75" customHeight="1">
       <c r="A699" s="1">
         <v>41597</v>
       </c>
@@ -34886,8 +35457,11 @@
       <c r="O699">
         <v>2</v>
       </c>
-    </row>
-    <row r="700" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P699">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="700" spans="1:16" ht="12.75" customHeight="1">
       <c r="A700" s="1">
         <v>41611</v>
       </c>
@@ -34933,8 +35507,11 @@
       <c r="O700">
         <v>2</v>
       </c>
-    </row>
-    <row r="701" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P700">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="701" spans="1:16" ht="12.75" customHeight="1">
       <c r="A701" s="1">
         <v>41625</v>
       </c>
@@ -34980,8 +35557,11 @@
       <c r="O701">
         <v>2</v>
       </c>
-    </row>
-    <row r="702" spans="1:15" ht="12.75" customHeight="1">
+      <c r="P701">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="702" spans="1:16" ht="12.75" customHeight="1">
       <c r="A702" s="1">
         <v>41635</v>
       </c>
@@ -35026,6 +35606,9 @@
       </c>
       <c r="O702">
         <v>2</v>
+      </c>
+      <c r="P702">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>